<commit_message>
Sarri 8elw na diavasw
</commit_message>
<xml_diff>
--- a/DataBase/Manos costs/costs.xlsx
+++ b/DataBase/Manos costs/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4201" uniqueCount="798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4216" uniqueCount="799">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -2408,6 +2408,9 @@
   </si>
   <si>
     <t>κρουασάν σοκολάτας</t>
+  </si>
+  <si>
+    <t>2 Σκεπαστές νηστήσιμες</t>
   </si>
 </sst>
 </file>
@@ -2559,7 +2562,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:J838" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:J841" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="10">
     <tableColumn id="1" name="amount" headerRowDxfId="10" totalsRowDxfId="9"/>
     <tableColumn id="11" name="type" totalsRowDxfId="8"/>
@@ -2861,10 +2864,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L838"/>
+  <dimension ref="A1:L841"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G833" workbookViewId="0">
-      <selection activeCell="J839" sqref="J839"/>
+    <sheetView tabSelected="1" topLeftCell="B833" workbookViewId="0">
+      <selection activeCell="J842" sqref="J842"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -27317,7 +27320,7 @@
         <v>207</v>
       </c>
       <c r="C837" s="7">
-        <v>43559</v>
+        <v>43558</v>
       </c>
       <c r="D837" s="1" t="s">
         <v>692</v>
@@ -27347,7 +27350,7 @@
         <v>207</v>
       </c>
       <c r="C838" s="7">
-        <v>43559</v>
+        <v>43558</v>
       </c>
       <c r="D838" s="1" t="s">
         <v>797</v>
@@ -27367,6 +27370,96 @@
       </c>
       <c r="J838" s="1" t="s">
         <v>639</v>
+      </c>
+    </row>
+    <row r="839" spans="1:10">
+      <c r="A839" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B839" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C839" s="7">
+        <v>43559</v>
+      </c>
+      <c r="D839" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="E839" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F839" s="1">
+        <v>5</v>
+      </c>
+      <c r="G839" s="1"/>
+      <c r="H839" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="I839" s="1">
+        <v>837</v>
+      </c>
+      <c r="J839" s="1" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="840" spans="1:10">
+      <c r="A840" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B840" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C840" s="7">
+        <v>43559</v>
+      </c>
+      <c r="D840" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="E840" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F840" s="1">
+        <v>5</v>
+      </c>
+      <c r="G840" s="1"/>
+      <c r="H840" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="I840" s="1">
+        <v>838</v>
+      </c>
+      <c r="J840" s="1" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="841" spans="1:10">
+      <c r="A841" s="1">
+        <v>9</v>
+      </c>
+      <c r="B841" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C841" s="7">
+        <v>43560</v>
+      </c>
+      <c r="D841" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="E841" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F841" s="1">
+        <v>5</v>
+      </c>
+      <c r="G841" s="1"/>
+      <c r="H841" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I841" s="1">
+        <v>839</v>
+      </c>
+      <c r="J841" s="1" t="s">
+        <v>648</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update database in Stavros Niarchos
</commit_message>
<xml_diff>
--- a/DataBase/Manos costs/costs.xlsx
+++ b/DataBase/Manos costs/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4316" uniqueCount="816">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4326" uniqueCount="818">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -2462,6 +2462,12 @@
   </si>
   <si>
     <t xml:space="preserve">pancake με σοκολάτα στο apolis με Κώστα Κούρο Σπύρο και Σοφιανό </t>
+  </si>
+  <si>
+    <t>ζελεδάκια και pizzetti με ντομάτα</t>
+  </si>
+  <si>
+    <t>coca cola light</t>
   </si>
 </sst>
 </file>
@@ -2613,7 +2619,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:J861" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:J863" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="10">
     <tableColumn id="1" name="amount" headerRowDxfId="10" totalsRowDxfId="9"/>
     <tableColumn id="11" name="type" totalsRowDxfId="8"/>
@@ -2915,10 +2921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L861"/>
+  <dimension ref="A1:L863"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B840" workbookViewId="0">
-      <selection activeCell="I862" sqref="I862"/>
+    <sheetView tabSelected="1" topLeftCell="A840" workbookViewId="0">
+      <selection activeCell="A864" sqref="A864"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -28112,6 +28118,66 @@
         <v>640</v>
       </c>
     </row>
+    <row r="862" spans="1:10">
+      <c r="A862" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B862" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C862" s="7">
+        <v>43579</v>
+      </c>
+      <c r="D862" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="E862" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F862" s="1">
+        <v>5</v>
+      </c>
+      <c r="G862" s="1"/>
+      <c r="H862" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I862" s="1">
+        <v>860</v>
+      </c>
+      <c r="J862" s="1" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="863" spans="1:10">
+      <c r="A863" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B863" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C863" s="7">
+        <v>43579</v>
+      </c>
+      <c r="D863" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="E863" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F863" s="1">
+        <v>5</v>
+      </c>
+      <c r="G863" s="1"/>
+      <c r="H863" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I863" s="1">
+        <v>861</v>
+      </c>
+      <c r="J863" s="1" t="s">
+        <v>638</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update costs in Tre Jolie
</commit_message>
<xml_diff>
--- a/DataBase/Manos costs/costs.xlsx
+++ b/DataBase/Manos costs/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4341" uniqueCount="819">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4346" uniqueCount="819">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -2622,7 +2622,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:J866" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:J867" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="10">
     <tableColumn id="1" name="amount" headerRowDxfId="10" totalsRowDxfId="9"/>
     <tableColumn id="11" name="type" totalsRowDxfId="8"/>
@@ -2924,10 +2924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L866"/>
+  <dimension ref="A1:L867"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B844" workbookViewId="0">
-      <selection activeCell="J867" sqref="J867"/>
+    <sheetView tabSelected="1" topLeftCell="A849" workbookViewId="0">
+      <selection activeCell="A868" sqref="A868"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -28271,6 +28271,36 @@
         <v>638</v>
       </c>
     </row>
+    <row r="867" spans="1:10">
+      <c r="A867" s="1">
+        <v>3.9</v>
+      </c>
+      <c r="B867" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C867" s="7">
+        <v>43586</v>
+      </c>
+      <c r="D867" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="E867" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F867" s="1">
+        <v>5</v>
+      </c>
+      <c r="G867" s="1"/>
+      <c r="H867" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I867" s="1">
+        <v>865</v>
+      </c>
+      <c r="J867" s="1" t="s">
+        <v>638</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Stavros niarchos me Kosta kai konne
</commit_message>
<xml_diff>
--- a/DataBase/Manos costs/costs.xlsx
+++ b/DataBase/Manos costs/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4346" uniqueCount="819">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4351" uniqueCount="820">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -2471,6 +2471,9 @@
   </si>
   <si>
     <t>hell και pizzetti</t>
+  </si>
+  <si>
+    <t>2 κουλούρια με ντομάτα και ελιά</t>
   </si>
 </sst>
 </file>
@@ -2622,7 +2625,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:J867" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:J868" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="10">
     <tableColumn id="1" name="amount" headerRowDxfId="10" totalsRowDxfId="9"/>
     <tableColumn id="11" name="type" totalsRowDxfId="8"/>
@@ -2924,10 +2927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L867"/>
+  <dimension ref="A1:L868"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A849" workbookViewId="0">
-      <selection activeCell="A868" sqref="A868"/>
+      <selection activeCell="A869" sqref="A869"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -28301,6 +28304,36 @@
         <v>638</v>
       </c>
     </row>
+    <row r="868" spans="1:10">
+      <c r="A868" s="1">
+        <v>3.8</v>
+      </c>
+      <c r="B868" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C868" s="7">
+        <v>43587</v>
+      </c>
+      <c r="D868" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="E868" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F868" s="1">
+        <v>5</v>
+      </c>
+      <c r="G868" s="1"/>
+      <c r="H868" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="I868" s="1">
+        <v>866</v>
+      </c>
+      <c r="J868" s="1" t="s">
+        <v>638</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Irthe Kostaras apo Larisa
</commit_message>
<xml_diff>
--- a/DataBase/Manos costs/costs.xlsx
+++ b/DataBase/Manos costs/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4541" uniqueCount="846">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4551" uniqueCount="848">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -2552,6 +2552,12 @@
   </si>
   <si>
     <t>bakerolls</t>
+  </si>
+  <si>
+    <t>parking στο penaroubia</t>
+  </si>
+  <si>
+    <t>strawberri smoothie</t>
   </si>
 </sst>
 </file>
@@ -2703,7 +2709,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:J906" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:J908" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="10">
     <tableColumn id="1" name="amount" headerRowDxfId="10" totalsRowDxfId="9"/>
     <tableColumn id="11" name="type" totalsRowDxfId="8"/>
@@ -3005,10 +3011,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L906"/>
+  <dimension ref="A1:L908"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B883" workbookViewId="0">
-      <selection activeCell="J907" sqref="J907"/>
+    <sheetView tabSelected="1" topLeftCell="B885" workbookViewId="0">
+      <selection activeCell="J909" sqref="J909"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -29552,6 +29558,66 @@
         <v>638</v>
       </c>
     </row>
+    <row r="907" spans="1:10">
+      <c r="A907" s="1">
+        <v>6</v>
+      </c>
+      <c r="B907" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C907" s="7">
+        <v>43613</v>
+      </c>
+      <c r="D907" s="1" t="s">
+        <v>847</v>
+      </c>
+      <c r="E907" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F907" s="1">
+        <v>5</v>
+      </c>
+      <c r="G907" s="1"/>
+      <c r="H907" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="I907" s="1">
+        <v>905</v>
+      </c>
+      <c r="J907" s="1" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="908" spans="1:10">
+      <c r="A908" s="1">
+        <v>5</v>
+      </c>
+      <c r="B908" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="C908" s="7">
+        <v>43613</v>
+      </c>
+      <c r="D908" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="E908" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F908" s="1">
+        <v>5</v>
+      </c>
+      <c r="G908" s="1"/>
+      <c r="H908" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="I908" s="1">
+        <v>906</v>
+      </c>
+      <c r="J908" s="1" t="s">
+        <v>638</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update with gus kala in Larissa
</commit_message>
<xml_diff>
--- a/DataBase/Manos costs/costs.xlsx
+++ b/DataBase/Manos costs/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4676" uniqueCount="868">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4711" uniqueCount="875">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -2618,6 +2618,27 @@
   </si>
   <si>
     <t>Attiki</t>
+  </si>
+  <si>
+    <t>ταξί από το σπίτι προς Ανθούπολη</t>
+  </si>
+  <si>
+    <t>τσίχλες στο τρένο</t>
+  </si>
+  <si>
+    <t>σαλάτα χανιώτικη από το Κρητικό περιβόλι</t>
+  </si>
+  <si>
+    <t>2 κομμάτα πίτσα</t>
+  </si>
+  <si>
+    <t>hell και μπουκαλάκι νερό</t>
+  </si>
+  <si>
+    <t>πίτσες και sprite στο Cosmos με Μποτσκαρίοφ team</t>
+  </si>
+  <si>
+    <t>3 μεγάλα νερά και 1 sprite</t>
   </si>
 </sst>
 </file>
@@ -2745,15 +2766,15 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2769,9 +2790,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:J933" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:J940" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="10">
-    <tableColumn id="1" name="amount" headerRowDxfId="9" totalsRowDxfId="10"/>
+    <tableColumn id="1" name="amount" headerRowDxfId="10" totalsRowDxfId="9"/>
     <tableColumn id="11" name="type" totalsRowDxfId="8"/>
     <tableColumn id="2" name="date" totalsRowDxfId="7"/>
     <tableColumn id="4" name="description" totalsRowDxfId="6"/>
@@ -3071,10 +3092,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L933"/>
+  <dimension ref="A1:L940"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A915" workbookViewId="0">
-      <selection activeCell="A934" sqref="A934"/>
+    <sheetView tabSelected="1" topLeftCell="B930" workbookViewId="0">
+      <selection activeCell="I941" sqref="I941"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -30427,6 +30448,216 @@
         <v>640</v>
       </c>
     </row>
+    <row r="934" spans="1:10">
+      <c r="A934" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="B934" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C934" s="7">
+        <v>43631</v>
+      </c>
+      <c r="D934" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="E934" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F934" s="1">
+        <v>5</v>
+      </c>
+      <c r="G934" s="1"/>
+      <c r="H934" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I934" s="1">
+        <v>932</v>
+      </c>
+      <c r="J934" s="1" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="935" spans="1:10">
+      <c r="A935" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B935" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C935" s="7">
+        <v>43631</v>
+      </c>
+      <c r="D935" s="1" t="s">
+        <v>869</v>
+      </c>
+      <c r="E935" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F935" s="1">
+        <v>5</v>
+      </c>
+      <c r="G935" s="1"/>
+      <c r="H935" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="I935" s="1">
+        <v>933</v>
+      </c>
+      <c r="J935" s="1" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="936" spans="1:10">
+      <c r="A936" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="B936" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C936" s="7">
+        <v>43631</v>
+      </c>
+      <c r="D936" s="1" t="s">
+        <v>870</v>
+      </c>
+      <c r="E936" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F936" s="1">
+        <v>5</v>
+      </c>
+      <c r="G936" s="1"/>
+      <c r="H936" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="I936" s="1">
+        <v>934</v>
+      </c>
+      <c r="J936" s="1" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="937" spans="1:10">
+      <c r="A937" s="1">
+        <v>2</v>
+      </c>
+      <c r="B937" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C937" s="7">
+        <v>43631</v>
+      </c>
+      <c r="D937" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="E937" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F937" s="1">
+        <v>5</v>
+      </c>
+      <c r="G937" s="1"/>
+      <c r="H937" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="I937" s="1">
+        <v>935</v>
+      </c>
+      <c r="J937" s="1" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="938" spans="1:10">
+      <c r="A938" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="B938" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C938" s="7">
+        <v>43631</v>
+      </c>
+      <c r="D938" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="E938" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F938" s="1">
+        <v>5</v>
+      </c>
+      <c r="G938" s="1"/>
+      <c r="H938" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="I938" s="1">
+        <v>936</v>
+      </c>
+      <c r="J938" s="1" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="939" spans="1:10">
+      <c r="A939" s="1">
+        <v>10</v>
+      </c>
+      <c r="B939" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C939" s="7">
+        <v>43631</v>
+      </c>
+      <c r="D939" s="1" t="s">
+        <v>873</v>
+      </c>
+      <c r="E939" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F939" s="1">
+        <v>5</v>
+      </c>
+      <c r="G939" s="1"/>
+      <c r="H939" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="I939" s="1">
+        <v>937</v>
+      </c>
+      <c r="J939" s="1" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="940" spans="1:10">
+      <c r="A940" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="B940" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C940" s="7">
+        <v>43631</v>
+      </c>
+      <c r="D940" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="E940" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F940" s="1">
+        <v>5</v>
+      </c>
+      <c r="G940" s="1"/>
+      <c r="H940" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="I940" s="1">
+        <v>938</v>
+      </c>
+      <c r="J940" s="1" t="s">
+        <v>638</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
first commit after FUCKING FORMAT
</commit_message>
<xml_diff>
--- a/DataBase/Manos costs/costs.xlsx
+++ b/DataBase/Manos costs/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4936" uniqueCount="907">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5036" uniqueCount="924">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -2735,6 +2735,57 @@
   </si>
   <si>
     <t>Alimos</t>
+  </si>
+  <si>
+    <t>στρίφωμα για το παντελόνι που μου πήρε η Μανούλα</t>
+  </si>
+  <si>
+    <t>ASC colostrum</t>
+  </si>
+  <si>
+    <t>φασόλια κονσέρβα str8 και ice tea φακελάκια</t>
+  </si>
+  <si>
+    <t>τυρόπιτα και κρουασάν σοκολάτας στο Απολλώνιον</t>
+  </si>
+  <si>
+    <t>6αδα νερά από τον Κρητικό</t>
+  </si>
+  <si>
+    <t>μπύρα με Καλλιοτζίδια στον καφενέ</t>
+  </si>
+  <si>
+    <t>amarretti από την Δέγλερη</t>
+  </si>
+  <si>
+    <t>κουλούρι με ελία και ντομάτα</t>
+  </si>
+  <si>
+    <t>coca-cola</t>
+  </si>
+  <si>
+    <t>σερμπετόσπιτο με Καρβουνίδη</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ice tea και πεϊνιρλί </t>
+  </si>
+  <si>
+    <t>vegan burger με καλλιοτζιδια στα simply</t>
+  </si>
+  <si>
+    <t>διόδια για να πάω στην Καρβουνίδη</t>
+  </si>
+  <si>
+    <t>μπύρες πατατάκια caprice (+ καρβουνίδη)</t>
+  </si>
+  <si>
+    <t>Dionyssos</t>
+  </si>
+  <si>
+    <t>φρουτοσαλάτα με παγωτό στο Άλσος με Αντώνη</t>
+  </si>
+  <si>
+    <t>ζελεδάκια</t>
   </si>
 </sst>
 </file>
@@ -2886,7 +2937,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:J985" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:J1005" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="10">
     <tableColumn id="1" name="amount" headerRowDxfId="10" totalsRowDxfId="9"/>
     <tableColumn id="11" name="type" totalsRowDxfId="8"/>
@@ -3188,10 +3239,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L985"/>
+  <dimension ref="A1:L1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B982" workbookViewId="0">
-      <selection activeCell="J986" sqref="J986"/>
+    <sheetView tabSelected="1" topLeftCell="A982" workbookViewId="0">
+      <selection activeCell="A1006" sqref="A1006"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -32102,6 +32153,532 @@
         <v>637</v>
       </c>
     </row>
+    <row r="986" spans="1:10">
+      <c r="A986" s="1">
+        <v>5</v>
+      </c>
+      <c r="B986" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C986" s="7">
+        <v>43651</v>
+      </c>
+      <c r="D986" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="E986" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F986" s="1">
+        <v>5</v>
+      </c>
+      <c r="G986" s="1"/>
+      <c r="H986" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I986" s="1"/>
+      <c r="J986" s="1" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="987" spans="1:10">
+      <c r="A987">
+        <v>71.98</v>
+      </c>
+      <c r="B987" t="s">
+        <v>322</v>
+      </c>
+      <c r="C987" s="2">
+        <v>43652</v>
+      </c>
+      <c r="D987" t="s">
+        <v>908</v>
+      </c>
+      <c r="E987" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F987">
+        <v>5</v>
+      </c>
+      <c r="H987" t="s">
+        <v>224</v>
+      </c>
+      <c r="J987" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="988" spans="1:10">
+      <c r="A988">
+        <v>5.95</v>
+      </c>
+      <c r="B988" t="s">
+        <v>207</v>
+      </c>
+      <c r="C988" s="2">
+        <v>43652</v>
+      </c>
+      <c r="D988" t="s">
+        <v>909</v>
+      </c>
+      <c r="E988" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F988">
+        <v>5</v>
+      </c>
+      <c r="H988" t="s">
+        <v>224</v>
+      </c>
+      <c r="J988" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="989" spans="1:10">
+      <c r="A989">
+        <v>0.99</v>
+      </c>
+      <c r="B989" t="s">
+        <v>207</v>
+      </c>
+      <c r="C989" s="2">
+        <v>43652</v>
+      </c>
+      <c r="D989" t="s">
+        <v>911</v>
+      </c>
+      <c r="E989" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F989">
+        <v>4</v>
+      </c>
+      <c r="H989" t="s">
+        <v>224</v>
+      </c>
+      <c r="J989" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="990" spans="1:10">
+      <c r="A990">
+        <v>3.4</v>
+      </c>
+      <c r="B990" t="s">
+        <v>207</v>
+      </c>
+      <c r="C990" s="2"/>
+      <c r="D990" t="s">
+        <v>910</v>
+      </c>
+      <c r="E990" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F990">
+        <v>5</v>
+      </c>
+      <c r="H990" t="s">
+        <v>371</v>
+      </c>
+      <c r="J990" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="991" spans="1:10">
+      <c r="A991">
+        <v>3</v>
+      </c>
+      <c r="B991" t="s">
+        <v>207</v>
+      </c>
+      <c r="C991" s="2">
+        <v>43653</v>
+      </c>
+      <c r="D991" t="s">
+        <v>912</v>
+      </c>
+      <c r="E991" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F991">
+        <v>5</v>
+      </c>
+      <c r="H991" t="s">
+        <v>399</v>
+      </c>
+      <c r="J991" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="992" spans="1:10">
+      <c r="A992">
+        <v>1.5</v>
+      </c>
+      <c r="B992" t="s">
+        <v>207</v>
+      </c>
+      <c r="C992" s="2">
+        <v>43653</v>
+      </c>
+      <c r="D992" t="s">
+        <v>913</v>
+      </c>
+      <c r="E992" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F992">
+        <v>5</v>
+      </c>
+      <c r="H992" t="s">
+        <v>224</v>
+      </c>
+      <c r="J992" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="993" spans="1:10">
+      <c r="A993">
+        <v>1.8</v>
+      </c>
+      <c r="B993" t="s">
+        <v>207</v>
+      </c>
+      <c r="C993" s="2">
+        <v>43654</v>
+      </c>
+      <c r="D993" t="s">
+        <v>914</v>
+      </c>
+      <c r="E993" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F993">
+        <v>4</v>
+      </c>
+      <c r="H993" t="s">
+        <v>231</v>
+      </c>
+      <c r="J993" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="994" spans="1:10">
+      <c r="A994">
+        <v>1.2</v>
+      </c>
+      <c r="B994" t="s">
+        <v>207</v>
+      </c>
+      <c r="C994" s="2">
+        <v>43654</v>
+      </c>
+      <c r="D994" t="s">
+        <v>915</v>
+      </c>
+      <c r="E994" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F994">
+        <v>4</v>
+      </c>
+      <c r="H994" t="s">
+        <v>231</v>
+      </c>
+      <c r="J994" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="995" spans="1:10">
+      <c r="A995">
+        <v>7</v>
+      </c>
+      <c r="B995" t="s">
+        <v>207</v>
+      </c>
+      <c r="C995" s="2">
+        <v>43654</v>
+      </c>
+      <c r="D995" t="s">
+        <v>916</v>
+      </c>
+      <c r="E995" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F995">
+        <v>5</v>
+      </c>
+      <c r="H995" t="s">
+        <v>229</v>
+      </c>
+      <c r="J995" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="996" spans="1:10">
+      <c r="A996">
+        <v>45.13</v>
+      </c>
+      <c r="B996" t="s">
+        <v>328</v>
+      </c>
+      <c r="C996" s="2">
+        <v>43655</v>
+      </c>
+      <c r="D996" t="s">
+        <v>772</v>
+      </c>
+      <c r="E996" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F996">
+        <v>5</v>
+      </c>
+      <c r="H996" t="s">
+        <v>224</v>
+      </c>
+      <c r="J996" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="997" spans="1:10">
+      <c r="A997">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B997" t="s">
+        <v>207</v>
+      </c>
+      <c r="C997" s="2">
+        <v>43656</v>
+      </c>
+      <c r="D997" t="s">
+        <v>917</v>
+      </c>
+      <c r="E997" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F997">
+        <v>5</v>
+      </c>
+      <c r="H997" t="s">
+        <v>231</v>
+      </c>
+      <c r="J997" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="998" spans="1:10">
+      <c r="A998">
+        <v>1</v>
+      </c>
+      <c r="B998" t="s">
+        <v>207</v>
+      </c>
+      <c r="C998" s="2">
+        <v>43656</v>
+      </c>
+      <c r="D998" t="s">
+        <v>337</v>
+      </c>
+      <c r="E998" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F998">
+        <v>5</v>
+      </c>
+      <c r="H998" t="s">
+        <v>231</v>
+      </c>
+      <c r="J998" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="999" spans="1:10">
+      <c r="A999">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B999" t="s">
+        <v>207</v>
+      </c>
+      <c r="C999" s="2">
+        <v>43656</v>
+      </c>
+      <c r="D999" t="s">
+        <v>918</v>
+      </c>
+      <c r="E999" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F999">
+        <v>5</v>
+      </c>
+      <c r="H999" t="s">
+        <v>255</v>
+      </c>
+      <c r="J999" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:10">
+      <c r="A1000">
+        <v>3.5</v>
+      </c>
+      <c r="B1000" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1000" s="2">
+        <v>43658</v>
+      </c>
+      <c r="D1000" t="s">
+        <v>306</v>
+      </c>
+      <c r="E1000" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1000">
+        <v>5</v>
+      </c>
+      <c r="H1000" t="s">
+        <v>224</v>
+      </c>
+      <c r="J1000" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:10">
+      <c r="A1001">
+        <v>10</v>
+      </c>
+      <c r="B1001" t="s">
+        <v>206</v>
+      </c>
+      <c r="C1001" s="2">
+        <v>43658</v>
+      </c>
+      <c r="D1001" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1001" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1001">
+        <v>5</v>
+      </c>
+      <c r="H1001" t="s">
+        <v>224</v>
+      </c>
+      <c r="J1001" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:10">
+      <c r="A1002">
+        <v>2.8</v>
+      </c>
+      <c r="B1002" t="s">
+        <v>330</v>
+      </c>
+      <c r="C1002" s="2">
+        <v>43659</v>
+      </c>
+      <c r="D1002" t="s">
+        <v>919</v>
+      </c>
+      <c r="E1002" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1002">
+        <v>5</v>
+      </c>
+      <c r="H1002" t="s">
+        <v>227</v>
+      </c>
+      <c r="J1002" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:10">
+      <c r="A1003" s="1">
+        <v>10</v>
+      </c>
+      <c r="B1003" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1003" s="2">
+        <v>43659</v>
+      </c>
+      <c r="D1003" s="1" t="s">
+        <v>920</v>
+      </c>
+      <c r="E1003" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1003" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1003" s="1"/>
+      <c r="H1003" s="1" t="s">
+        <v>921</v>
+      </c>
+      <c r="I1003" s="1"/>
+      <c r="J1003" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:10">
+      <c r="A1004" s="1">
+        <v>6</v>
+      </c>
+      <c r="B1004" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1004" s="2">
+        <v>43660</v>
+      </c>
+      <c r="D1004" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="E1004" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1004" s="1">
+        <v>4</v>
+      </c>
+      <c r="G1004" s="1"/>
+      <c r="H1004" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1004" s="1"/>
+      <c r="J1004" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:10">
+      <c r="A1005" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B1005" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1005" s="7">
+        <v>43660</v>
+      </c>
+      <c r="D1005" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="E1005" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1005" s="1">
+        <v>4</v>
+      </c>
+      <c r="G1005" s="1"/>
+      <c r="H1005" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1005" s="1"/>
+      <c r="J1005" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Tous Kwdikous tou UDEMY opote mporeis :-)
</commit_message>
<xml_diff>
--- a/DataBase/Manos costs/costs.xlsx
+++ b/DataBase/Manos costs/costs.xlsx
@@ -3268,8 +3268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L1019"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1010" workbookViewId="0">
-      <selection activeCell="J1020" sqref="J1020"/>
+    <sheetView tabSelected="1" topLeftCell="B997" workbookViewId="0">
+      <selection activeCell="I1020" sqref="I1020"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -32094,36 +32094,33 @@
       <c r="A983" s="1">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B983" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="C983" s="7">
+      <c r="B983" t="s">
+        <v>207</v>
+      </c>
+      <c r="C983" s="2">
         <v>43649</v>
       </c>
-      <c r="D983" s="1" t="s">
-        <v>904</v>
+      <c r="D983" t="s">
+        <v>910</v>
       </c>
       <c r="E983" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="F983" s="1">
-        <v>5</v>
-      </c>
-      <c r="G983" s="1"/>
-      <c r="H983" s="1" t="s">
-        <v>231</v>
+      <c r="F983">
+        <v>5</v>
+      </c>
+      <c r="H983" t="s">
+        <v>371</v>
       </c>
       <c r="I983" s="1">
         <v>981</v>
       </c>
-      <c r="J983" s="1" t="s">
-        <v>637</v>
+      <c r="J983" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="984" spans="1:10">
-      <c r="A984" s="1">
-        <v>0.5</v>
-      </c>
+      <c r="A984" s="1"/>
       <c r="B984" s="1" t="s">
         <v>207</v>
       </c>
@@ -32131,7 +32128,7 @@
         <v>43649</v>
       </c>
       <c r="D984" s="1" t="s">
-        <v>76</v>
+        <v>904</v>
       </c>
       <c r="E984" s="1" t="s">
         <v>220</v>
@@ -32152,16 +32149,16 @@
     </row>
     <row r="985" spans="1:10">
       <c r="A985" s="1">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="B985" s="1" t="s">
         <v>207</v>
       </c>
       <c r="C985" s="7">
-        <v>43650</v>
+        <v>43649</v>
       </c>
       <c r="D985" s="1" t="s">
-        <v>905</v>
+        <v>76</v>
       </c>
       <c r="E985" s="1" t="s">
         <v>220</v>
@@ -32171,7 +32168,7 @@
       </c>
       <c r="G985" s="1"/>
       <c r="H985" s="1" t="s">
-        <v>906</v>
+        <v>231</v>
       </c>
       <c r="I985" s="1">
         <v>983</v>
@@ -32185,13 +32182,13 @@
         <v>5</v>
       </c>
       <c r="B986" s="1" t="s">
-        <v>321</v>
+        <v>207</v>
       </c>
       <c r="C986" s="7">
-        <v>43651</v>
+        <v>43650</v>
       </c>
       <c r="D986" s="1" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="E986" s="1" t="s">
         <v>220</v>
@@ -32201,56 +32198,57 @@
       </c>
       <c r="G986" s="1"/>
       <c r="H986" s="1" t="s">
-        <v>224</v>
+        <v>906</v>
       </c>
       <c r="I986" s="1">
         <v>984</v>
       </c>
       <c r="J986" s="1" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
     </row>
     <row r="987" spans="1:10">
-      <c r="A987">
-        <v>71.98</v>
-      </c>
-      <c r="B987" t="s">
-        <v>322</v>
-      </c>
-      <c r="C987" s="2">
-        <v>43652</v>
-      </c>
-      <c r="D987" t="s">
-        <v>908</v>
+      <c r="A987" s="1">
+        <v>5</v>
+      </c>
+      <c r="B987" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C987" s="7">
+        <v>43651</v>
+      </c>
+      <c r="D987" s="1" t="s">
+        <v>907</v>
       </c>
       <c r="E987" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="F987">
-        <v>5</v>
-      </c>
-      <c r="H987" t="s">
+      <c r="F987" s="1">
+        <v>5</v>
+      </c>
+      <c r="G987" s="1"/>
+      <c r="H987" s="1" t="s">
         <v>224</v>
       </c>
       <c r="I987" s="1">
         <v>985</v>
       </c>
-      <c r="J987" t="s">
+      <c r="J987" s="1" t="s">
         <v>639</v>
       </c>
     </row>
     <row r="988" spans="1:10">
       <c r="A988">
-        <v>5.95</v>
+        <v>71.98</v>
       </c>
       <c r="B988" t="s">
-        <v>207</v>
+        <v>322</v>
       </c>
       <c r="C988" s="2">
         <v>43652</v>
       </c>
       <c r="D988" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="E988" s="1" t="s">
         <v>220</v>
@@ -32270,7 +32268,7 @@
     </row>
     <row r="989" spans="1:10">
       <c r="A989">
-        <v>0.99</v>
+        <v>5.95</v>
       </c>
       <c r="B989" t="s">
         <v>207</v>
@@ -32279,13 +32277,13 @@
         <v>43652</v>
       </c>
       <c r="D989" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="E989" s="1" t="s">
         <v>220</v>
       </c>
       <c r="F989">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H989" t="s">
         <v>224</v>
@@ -32299,23 +32297,25 @@
     </row>
     <row r="990" spans="1:10">
       <c r="A990">
-        <v>3.4</v>
+        <v>0.99</v>
       </c>
       <c r="B990" t="s">
         <v>207</v>
       </c>
-      <c r="C990" s="2"/>
+      <c r="C990" s="2">
+        <v>43652</v>
+      </c>
       <c r="D990" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="E990" s="1" t="s">
         <v>220</v>
       </c>
       <c r="F990">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H990" t="s">
-        <v>371</v>
+        <v>224</v>
       </c>
       <c r="I990" s="1">
         <v>988</v>

</xml_diff>

<commit_message>
new video on YouTube
</commit_message>
<xml_diff>
--- a/DataBase/Manos costs/costs.xlsx
+++ b/DataBase/Manos costs/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5237" uniqueCount="962">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5322" uniqueCount="973">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -2857,9 +2857,6 @@
     <t>Σουβενίρ από Σκωτία</t>
   </si>
   <si>
-    <t>2,2.</t>
-  </si>
-  <si>
     <t>για την λευχαιμία</t>
   </si>
   <si>
@@ -2900,6 +2897,42 @@
   </si>
   <si>
     <t>(+ ταξί Νικολόπουλου)</t>
+  </si>
+  <si>
+    <t>(+ νερό Μιχάλη)</t>
+  </si>
+  <si>
+    <t>caprice capuccino και 2 τσαι του βουνού Όλυμπος</t>
+  </si>
+  <si>
+    <t>βενζίνη για το Yaris</t>
+  </si>
+  <si>
+    <t>μπύρες στο Bronco με Κώστα και Κωνσταντίνα</t>
+  </si>
+  <si>
+    <t>tonic water (+ μπύρα Κώστα)</t>
+  </si>
+  <si>
+    <t>εξετάσεις αίματος (+ πατέρα)</t>
+  </si>
+  <si>
+    <t>πεϊνιρλί (+ Μαρίας πουρνάρα)</t>
+  </si>
+  <si>
+    <t>για την τούρτα του Κώστα</t>
+  </si>
+  <si>
+    <t>λουκουμάς σταθμό Λαρίσσης</t>
+  </si>
+  <si>
+    <t>instagram views</t>
+  </si>
+  <si>
+    <t>instagram likes</t>
+  </si>
+  <si>
+    <t>instagram followers and likes</t>
   </si>
 </sst>
 </file>
@@ -3051,7 +3084,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:J1045" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:J1062" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="10">
     <tableColumn id="1" name="amount" headerRowDxfId="10" totalsRowDxfId="9"/>
     <tableColumn id="11" name="type" totalsRowDxfId="8"/>
@@ -3353,10 +3386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1045"/>
+  <dimension ref="A1:L1062"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1022" workbookViewId="0">
-      <selection activeCell="D1046" sqref="D1046"/>
+    <sheetView tabSelected="1" topLeftCell="B1044" workbookViewId="0">
+      <selection activeCell="J1063" sqref="J1063"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -33616,8 +33649,8 @@
       </c>
     </row>
     <row r="1032" spans="1:10">
-      <c r="A1032" s="1" t="s">
-        <v>947</v>
+      <c r="A1032" s="1">
+        <v>2.2000000000000002</v>
       </c>
       <c r="B1032" s="1" t="s">
         <v>549</v>
@@ -33626,7 +33659,7 @@
         <v>43671</v>
       </c>
       <c r="D1032" s="1" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="E1032" s="1" t="s">
         <v>221</v>
@@ -33644,13 +33677,17 @@
       </c>
     </row>
     <row r="1033" spans="1:10">
-      <c r="A1033" s="1"/>
-      <c r="B1033" s="1"/>
+      <c r="A1033" s="1">
+        <v>11</v>
+      </c>
+      <c r="B1033" s="1" t="s">
+        <v>207</v>
+      </c>
       <c r="C1033" s="7">
         <v>43671</v>
       </c>
       <c r="D1033" s="1" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="E1033" s="1" t="s">
         <v>221</v>
@@ -33668,7 +33705,9 @@
       </c>
     </row>
     <row r="1034" spans="1:10">
-      <c r="A1034" s="1"/>
+      <c r="A1034" s="1">
+        <v>25</v>
+      </c>
       <c r="B1034" s="1" t="s">
         <v>557</v>
       </c>
@@ -33676,7 +33715,7 @@
         <v>43671</v>
       </c>
       <c r="D1034" s="1" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="E1034" s="1" t="s">
         <v>221</v>
@@ -33704,7 +33743,7 @@
         <v>43671</v>
       </c>
       <c r="D1035" s="1" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="E1035" s="1" t="s">
         <v>221</v>
@@ -33714,7 +33753,7 @@
       </c>
       <c r="G1035" s="1"/>
       <c r="H1035" s="1" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="I1035" s="1"/>
       <c r="J1035" s="1" t="s">
@@ -33732,7 +33771,7 @@
         <v>43671</v>
       </c>
       <c r="D1036" s="1" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="E1036" s="1" t="s">
         <v>221</v>
@@ -33742,7 +33781,7 @@
       </c>
       <c r="G1036" s="1"/>
       <c r="H1036" s="1" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="I1036" s="1"/>
       <c r="J1036" s="1" t="s">
@@ -33760,7 +33799,7 @@
         <v>43672</v>
       </c>
       <c r="D1037" s="1" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="E1037" s="1" t="s">
         <v>221</v>
@@ -33770,7 +33809,7 @@
       </c>
       <c r="G1037" s="1"/>
       <c r="H1037" s="1" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="I1037" s="1"/>
       <c r="J1037" s="1" t="s">
@@ -33788,7 +33827,7 @@
         <v>43672</v>
       </c>
       <c r="D1038" s="1" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="E1038" s="1" t="s">
         <v>221</v>
@@ -33798,7 +33837,7 @@
       </c>
       <c r="G1038" s="1"/>
       <c r="H1038" s="1" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="I1038" s="1"/>
       <c r="J1038" s="1" t="s">
@@ -33816,7 +33855,7 @@
         <v>43672</v>
       </c>
       <c r="D1039" s="1" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="E1039" s="1" t="s">
         <v>221</v>
@@ -33826,7 +33865,7 @@
       </c>
       <c r="G1039" s="1"/>
       <c r="H1039" s="1" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="I1039" s="1"/>
       <c r="J1039" s="1" t="s">
@@ -33844,7 +33883,7 @@
         <v>43672</v>
       </c>
       <c r="D1040" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="E1040" s="1" t="s">
         <v>221</v>
@@ -33872,7 +33911,7 @@
         <v>43672</v>
       </c>
       <c r="D1041" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="E1041" s="1" t="s">
         <v>221</v>
@@ -33900,7 +33939,7 @@
         <v>43672</v>
       </c>
       <c r="D1042" s="1" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="E1042" s="1" t="s">
         <v>221</v>
@@ -33928,7 +33967,7 @@
         <v>43672</v>
       </c>
       <c r="D1043" s="1" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="E1043" s="1" t="s">
         <v>221</v>
@@ -33984,7 +34023,7 @@
         <v>43674</v>
       </c>
       <c r="D1045" s="1" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="E1045" s="1" t="s">
         <v>221</v>
@@ -33999,6 +34038,482 @@
       <c r="I1045" s="1"/>
       <c r="J1045" s="1" t="s">
         <v>637</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:10">
+      <c r="A1046" s="1">
+        <v>2</v>
+      </c>
+      <c r="B1046" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1046" s="7">
+        <v>43674</v>
+      </c>
+      <c r="D1046" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E1046" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1046" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1046" s="1"/>
+      <c r="H1046" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1046" s="1"/>
+      <c r="J1046" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:10">
+      <c r="A1047" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B1047" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1047" s="7">
+        <v>43674</v>
+      </c>
+      <c r="D1047" s="1" t="s">
+        <v>961</v>
+      </c>
+      <c r="E1047" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1047" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1047" s="1"/>
+      <c r="H1047" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1047" s="1"/>
+      <c r="J1047" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:10">
+      <c r="A1048" s="1">
+        <v>6.21</v>
+      </c>
+      <c r="B1048" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1048" s="7">
+        <v>43675</v>
+      </c>
+      <c r="D1048" s="1" t="s">
+        <v>962</v>
+      </c>
+      <c r="E1048" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1048" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1048" s="1"/>
+      <c r="H1048" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1048" s="1"/>
+      <c r="J1048" s="1" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:10">
+      <c r="A1049" s="1">
+        <v>20</v>
+      </c>
+      <c r="B1049" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C1049" s="7">
+        <v>43675</v>
+      </c>
+      <c r="D1049" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E1049" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1049" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1049" s="1"/>
+      <c r="H1049" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1049" s="1"/>
+      <c r="J1049" s="1" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:10">
+      <c r="A1050" s="1">
+        <v>7</v>
+      </c>
+      <c r="B1050" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1050" s="7">
+        <v>43676</v>
+      </c>
+      <c r="D1050" s="1" t="s">
+        <v>964</v>
+      </c>
+      <c r="E1050" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1050" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1050" s="1"/>
+      <c r="H1050" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="I1050" s="1"/>
+      <c r="J1050" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:10">
+      <c r="A1051" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="B1051" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1051" s="7">
+        <v>43676</v>
+      </c>
+      <c r="D1051" s="1" t="s">
+        <v>965</v>
+      </c>
+      <c r="E1051" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1051" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1051" s="1"/>
+      <c r="H1051" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="I1051" s="1"/>
+      <c r="J1051" s="1" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:10">
+      <c r="A1052" s="1">
+        <v>20</v>
+      </c>
+      <c r="B1052" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C1052" s="7">
+        <v>43676</v>
+      </c>
+      <c r="D1052" s="1" t="s">
+        <v>966</v>
+      </c>
+      <c r="E1052" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1052" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1052" s="1"/>
+      <c r="H1052" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="I1052" s="1"/>
+      <c r="J1052" s="1" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:10">
+      <c r="A1053" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="B1053" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1053" s="7">
+        <v>43676</v>
+      </c>
+      <c r="D1053" s="1" t="s">
+        <v>967</v>
+      </c>
+      <c r="E1053" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1053" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1053" s="1"/>
+      <c r="H1053" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="I1053" s="1"/>
+      <c r="J1053" s="1" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:10">
+      <c r="A1054" s="1">
+        <v>3</v>
+      </c>
+      <c r="B1054" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1054" s="7">
+        <v>43678</v>
+      </c>
+      <c r="D1054" s="1" t="s">
+        <v>968</v>
+      </c>
+      <c r="E1054" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1054" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1054" s="1"/>
+      <c r="H1054" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1054" s="1"/>
+      <c r="J1054" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:10">
+      <c r="A1055" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B1055" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1055" s="7">
+        <v>43678</v>
+      </c>
+      <c r="D1055" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E1055" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1055" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1055" s="1"/>
+      <c r="H1055" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1055" s="1"/>
+      <c r="J1055" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:10">
+      <c r="A1056" s="1">
+        <v>10</v>
+      </c>
+      <c r="B1056" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C1056" s="7">
+        <v>43678</v>
+      </c>
+      <c r="D1056" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1056" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1056" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1056" s="1"/>
+      <c r="H1056" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1056" s="1"/>
+      <c r="J1056" s="1" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:10">
+      <c r="A1057" s="1">
+        <v>1</v>
+      </c>
+      <c r="B1057" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1057" s="7">
+        <v>43678</v>
+      </c>
+      <c r="D1057" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="E1057" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1057" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1057" s="1"/>
+      <c r="H1057" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="I1057" s="1"/>
+      <c r="J1057" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:10">
+      <c r="A1058" s="1">
+        <v>20.329999999999998</v>
+      </c>
+      <c r="B1058" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="C1058" s="7">
+        <v>43679</v>
+      </c>
+      <c r="D1058" s="1" t="s">
+        <v>972</v>
+      </c>
+      <c r="E1058" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1058" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1058" s="1"/>
+      <c r="H1058" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="I1058" s="1"/>
+      <c r="J1058" s="1" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:10">
+      <c r="A1059" s="1">
+        <v>8.8699999999999992</v>
+      </c>
+      <c r="B1059" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="C1059" s="7">
+        <v>43679</v>
+      </c>
+      <c r="D1059" s="1" t="s">
+        <v>971</v>
+      </c>
+      <c r="E1059" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1059" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1059" s="1"/>
+      <c r="H1059" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="I1059" s="1"/>
+      <c r="J1059" s="1" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:10">
+      <c r="A1060" s="1">
+        <v>26.91</v>
+      </c>
+      <c r="B1060" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="C1060" s="7">
+        <v>43679</v>
+      </c>
+      <c r="D1060" s="1" t="s">
+        <v>971</v>
+      </c>
+      <c r="E1060" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1060" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1060" s="1"/>
+      <c r="H1060" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="I1060" s="1"/>
+      <c r="J1060" s="1" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:10">
+      <c r="A1061" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="B1061" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="C1061" s="7">
+        <v>43682</v>
+      </c>
+      <c r="D1061" s="1" t="s">
+        <v>970</v>
+      </c>
+      <c r="E1061" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1061" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1061" s="1"/>
+      <c r="H1061" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="I1061" s="1"/>
+      <c r="J1061" s="1" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:10">
+      <c r="A1062" s="1">
+        <v>1</v>
+      </c>
+      <c r="B1062" t="s">
+        <v>330</v>
+      </c>
+      <c r="C1062" s="2">
+        <v>43684</v>
+      </c>
+      <c r="D1062" t="s">
+        <v>444</v>
+      </c>
+      <c r="E1062" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1062" s="1">
+        <v>3</v>
+      </c>
+      <c r="G1062" s="1"/>
+      <c r="H1062" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="I1062" s="1"/>
+      <c r="J1062" s="1" t="s">
+        <v>646</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
H Ausrtia gamaei opws leei kai o filippou
</commit_message>
<xml_diff>
--- a/DataBase/Manos costs/costs.xlsx
+++ b/DataBase/Manos costs/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5497" uniqueCount="1006">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5602" uniqueCount="1023">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -3032,6 +3032,57 @@
   </si>
   <si>
     <t>2 falafel και 1 monster από τον Γρηγόρη Συγγρού</t>
+  </si>
+  <si>
+    <t>(+ coca-cola και τσιγάρα μανούλας)</t>
+  </si>
+  <si>
+    <t>καφές (+ Νίκου)</t>
+  </si>
+  <si>
+    <t>σοκοφρέτα (+ coca-cola Μαρίας)</t>
+  </si>
+  <si>
+    <t>οικολογικό σουβλάκι στο nesta</t>
+  </si>
+  <si>
+    <t>200 followers</t>
+  </si>
+  <si>
+    <t>κουλούρι με σοκολάτα, μπαστούνια τυριού, monster και καφέ από την σχολή</t>
+  </si>
+  <si>
+    <t>καφέ με Ζήση στο μπρίκι</t>
+  </si>
+  <si>
+    <t>τσάι ροδάκινο στην καφετέρια του Πανελληνίου</t>
+  </si>
+  <si>
+    <t>app για το κινητό</t>
+  </si>
+  <si>
+    <t>RFID reader και αδειες κάρτες</t>
+  </si>
+  <si>
+    <t>axe για τον άνδρα</t>
+  </si>
+  <si>
+    <t>τσάι του βουνού</t>
+  </si>
+  <si>
+    <t>καφές στην πλατεία Γεωργίου με Αγίλαρα βαγγελιώ και ξαδερφια</t>
+  </si>
+  <si>
+    <t>μπύρα radler και παγωτό με Νικηφόρο</t>
+  </si>
+  <si>
+    <t>κρουασάν βουτήρου Φουρναριό και τυρόπιτα από το κηλικείο σχολής</t>
+  </si>
+  <si>
+    <t>πατατάκια με πάπρικα</t>
+  </si>
+  <si>
+    <t>αεροπορικά για Βιέννη</t>
   </si>
 </sst>
 </file>
@@ -3183,7 +3234,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:J1097" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A2:J1118" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="10">
     <tableColumn id="1" name="amount" headerRowDxfId="10" totalsRowDxfId="9"/>
     <tableColumn id="11" name="type" totalsRowDxfId="8"/>
@@ -3485,10 +3536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1097"/>
+  <dimension ref="A1:L1118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1076" workbookViewId="0">
-      <selection activeCell="D1098" sqref="D1098"/>
+    <sheetView tabSelected="1" topLeftCell="C1100" workbookViewId="0">
+      <selection activeCell="I1096" sqref="I1096:I1118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3496,7 +3547,7 @@
     <col min="1" max="1" width="9.28515625" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="71.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.42578125" customWidth="1"/>
     <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -35735,6 +35786,636 @@
         <v>637</v>
       </c>
     </row>
+    <row r="1098" spans="1:10">
+      <c r="A1098" s="1">
+        <v>5.8</v>
+      </c>
+      <c r="B1098" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C1098" s="7">
+        <v>43706</v>
+      </c>
+      <c r="D1098" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="E1098" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1098" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1098" s="1"/>
+      <c r="H1098" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1098" s="1">
+        <v>1096</v>
+      </c>
+      <c r="J1098" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:10">
+      <c r="A1099" s="1">
+        <v>6</v>
+      </c>
+      <c r="B1099" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1099" s="7">
+        <v>43707</v>
+      </c>
+      <c r="D1099" s="1" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E1099" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1099" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1099" s="1"/>
+      <c r="H1099" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="I1099" s="1">
+        <v>1097</v>
+      </c>
+      <c r="J1099" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:10">
+      <c r="A1100" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B1100" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1100" s="7">
+        <v>43707</v>
+      </c>
+      <c r="D1100" s="1" t="s">
+        <v>1008</v>
+      </c>
+      <c r="E1100" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1100" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1100" s="1"/>
+      <c r="H1100" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="I1100" s="1">
+        <v>1098</v>
+      </c>
+      <c r="J1100" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:10">
+      <c r="A1101" s="1">
+        <v>1.9</v>
+      </c>
+      <c r="B1101" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1101" s="7">
+        <v>43707</v>
+      </c>
+      <c r="D1101" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="E1101" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1101" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1101" s="1"/>
+      <c r="H1101" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1101" s="1">
+        <v>1099</v>
+      </c>
+      <c r="J1101" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:10">
+      <c r="A1102" s="1">
+        <v>6.6</v>
+      </c>
+      <c r="B1102" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1102" s="7">
+        <v>43710</v>
+      </c>
+      <c r="D1102" s="1" t="s">
+        <v>1011</v>
+      </c>
+      <c r="E1102" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1102" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1102" s="1"/>
+      <c r="H1102" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="I1102" s="1">
+        <v>1100</v>
+      </c>
+      <c r="J1102" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:10">
+      <c r="A1103" s="1">
+        <v>3</v>
+      </c>
+      <c r="B1103" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1103" s="7">
+        <v>43710</v>
+      </c>
+      <c r="D1103" s="1" t="s">
+        <v>1012</v>
+      </c>
+      <c r="E1103" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1103" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1103" s="1"/>
+      <c r="H1103" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="I1103" s="1">
+        <v>1101</v>
+      </c>
+      <c r="J1103" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:10">
+      <c r="A1104" s="1">
+        <v>4.66</v>
+      </c>
+      <c r="B1104" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1104" s="7">
+        <v>43710</v>
+      </c>
+      <c r="D1104" s="1" t="s">
+        <v>1010</v>
+      </c>
+      <c r="E1104" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1104" s="1">
+        <v>4</v>
+      </c>
+      <c r="G1104" s="1"/>
+      <c r="H1104" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1104" s="1">
+        <v>1102</v>
+      </c>
+      <c r="J1104" s="1" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:10">
+      <c r="A1105" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B1105" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1105" s="7">
+        <v>43712</v>
+      </c>
+      <c r="D1105" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="E1105" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1105" s="1">
+        <v>4</v>
+      </c>
+      <c r="G1105" s="1"/>
+      <c r="H1105" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="I1105" s="1">
+        <v>1103</v>
+      </c>
+      <c r="J1105" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:10">
+      <c r="A1106" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="B1106" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1106" s="7">
+        <v>43712</v>
+      </c>
+      <c r="D1106" s="1" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E1106" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1106" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1106" s="1"/>
+      <c r="H1106" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="I1106" s="1">
+        <v>1104</v>
+      </c>
+      <c r="J1106" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:10">
+      <c r="A1107" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="B1107" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1107" s="7">
+        <v>43712</v>
+      </c>
+      <c r="D1107" s="1" t="s">
+        <v>986</v>
+      </c>
+      <c r="E1107" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1107" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1107" s="1"/>
+      <c r="H1107" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="I1107" s="1">
+        <v>1105</v>
+      </c>
+      <c r="J1107" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:10">
+      <c r="A1108" s="1">
+        <v>2.99</v>
+      </c>
+      <c r="B1108" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="C1108" s="7">
+        <v>43713</v>
+      </c>
+      <c r="D1108" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="E1108" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1108" s="1">
+        <v>4</v>
+      </c>
+      <c r="G1108" s="1"/>
+      <c r="H1108" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1108" s="1">
+        <v>1106</v>
+      </c>
+      <c r="J1108" s="1" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:10">
+      <c r="A1109" s="1">
+        <v>16</v>
+      </c>
+      <c r="B1109" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1109" s="7">
+        <v>43713</v>
+      </c>
+      <c r="D1109" s="1" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E1109" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1109" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1109" s="1"/>
+      <c r="H1109" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="I1109" s="1">
+        <v>1107</v>
+      </c>
+      <c r="J1109" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:10">
+      <c r="A1110" s="1">
+        <v>1.78</v>
+      </c>
+      <c r="B1110" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C1110" s="7">
+        <v>43713</v>
+      </c>
+      <c r="D1110" s="1" t="s">
+        <v>1017</v>
+      </c>
+      <c r="E1110" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1110" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1110" s="1"/>
+      <c r="H1110" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="I1110" s="1">
+        <v>1108</v>
+      </c>
+      <c r="J1110" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:10">
+      <c r="A1111" s="1">
+        <v>4</v>
+      </c>
+      <c r="B1111" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C1111" s="7">
+        <v>43713</v>
+      </c>
+      <c r="D1111" s="1" t="s">
+        <v>1016</v>
+      </c>
+      <c r="E1111" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1111" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1111" s="1"/>
+      <c r="H1111" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="I1111" s="1">
+        <v>1109</v>
+      </c>
+      <c r="J1111" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:10">
+      <c r="A1112" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="B1112" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1112" s="7">
+        <v>43713</v>
+      </c>
+      <c r="D1112" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E1112" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1112" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1112" s="1"/>
+      <c r="H1112" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="I1112" s="1">
+        <v>1110</v>
+      </c>
+      <c r="J1112" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:10">
+      <c r="A1113" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="B1113" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1113" s="7">
+        <v>43715</v>
+      </c>
+      <c r="D1113" s="1" t="s">
+        <v>1018</v>
+      </c>
+      <c r="E1113" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1113" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1113" s="1"/>
+      <c r="H1113" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="I1113" s="1">
+        <v>1111</v>
+      </c>
+      <c r="J1113" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:10">
+      <c r="A1114" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B1114" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1114" s="7">
+        <v>43716</v>
+      </c>
+      <c r="D1114" s="1" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E1114" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1114" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1114" s="1"/>
+      <c r="H1114" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1114" s="1">
+        <v>1112</v>
+      </c>
+      <c r="J1114" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:10">
+      <c r="A1115" s="1">
+        <v>1.9</v>
+      </c>
+      <c r="B1115" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1115" s="7">
+        <v>43718</v>
+      </c>
+      <c r="D1115" s="1" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E1115" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1115" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1115" s="1"/>
+      <c r="H1115" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="I1115" s="1">
+        <v>1113</v>
+      </c>
+      <c r="J1115" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:10">
+      <c r="A1116" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="B1116" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1116" s="7">
+        <v>43718</v>
+      </c>
+      <c r="D1116" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="E1116" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1116" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1116" s="1"/>
+      <c r="H1116" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1116" s="1">
+        <v>1114</v>
+      </c>
+      <c r="J1116" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:10">
+      <c r="A1117" s="1">
+        <v>57</v>
+      </c>
+      <c r="B1117" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C1117" s="7">
+        <v>43718</v>
+      </c>
+      <c r="D1117" s="1" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E1117" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1117" s="1">
+        <v>4</v>
+      </c>
+      <c r="G1117" s="1"/>
+      <c r="H1117" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1117" s="1">
+        <v>1115</v>
+      </c>
+      <c r="J1117" s="1" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:10">
+      <c r="A1118" s="1">
+        <v>29.98</v>
+      </c>
+      <c r="B1118" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C1118" s="7">
+        <v>43718</v>
+      </c>
+      <c r="D1118" s="1" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E1118" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1118" s="1">
+        <v>4</v>
+      </c>
+      <c r="G1118" s="1"/>
+      <c r="H1118" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1118" s="1">
+        <v>1116</v>
+      </c>
+      <c r="J1118" s="1" t="s">
+        <v>646</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
esvisa ta video katala8os
</commit_message>
<xml_diff>
--- a/DataBase/Manos costs/costs.xlsx
+++ b/DataBase/Manos costs/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5777" uniqueCount="1051">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5797" uniqueCount="1055">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -3167,6 +3167,18 @@
   </si>
   <si>
     <t>πίτσα και γραβιερόπιτα από την victoria</t>
+  </si>
+  <si>
+    <t>παπούτσια άρσης βαρών</t>
+  </si>
+  <si>
+    <t>αμύγδαλα καρύδια και πουράκια caprice με capuchino</t>
+  </si>
+  <si>
+    <t>(+ Σουβλάκια μανούλας)</t>
+  </si>
+  <si>
+    <t>vegeterian burger με ανανά με Νικολόπουλο και Ελίνα</t>
   </si>
 </sst>
 </file>
@@ -3620,10 +3632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1153"/>
+  <dimension ref="A1:L1157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1139" workbookViewId="0">
-      <selection activeCell="H1154" sqref="H1154"/>
+    <sheetView tabSelected="1" topLeftCell="C1149" workbookViewId="0">
+      <selection activeCell="I1152" sqref="I1152:I1157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -37535,6 +37547,122 @@
         <v>639</v>
       </c>
     </row>
+    <row r="1154" spans="1:10">
+      <c r="A1154">
+        <v>14.93</v>
+      </c>
+      <c r="B1154" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1154" s="2">
+        <v>43750</v>
+      </c>
+      <c r="D1154" t="s">
+        <v>1052</v>
+      </c>
+      <c r="E1154" t="s">
+        <v>222</v>
+      </c>
+      <c r="F1154">
+        <v>5</v>
+      </c>
+      <c r="H1154" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1154">
+        <v>1152</v>
+      </c>
+      <c r="J1154" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1155" spans="1:10">
+      <c r="A1155">
+        <v>44.98</v>
+      </c>
+      <c r="B1155" t="s">
+        <v>321</v>
+      </c>
+      <c r="C1155" s="2">
+        <v>43751</v>
+      </c>
+      <c r="D1155" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E1155" t="s">
+        <v>222</v>
+      </c>
+      <c r="F1155">
+        <v>5</v>
+      </c>
+      <c r="H1155" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1155">
+        <v>1153</v>
+      </c>
+      <c r="J1155" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:10">
+      <c r="A1156">
+        <v>10.8</v>
+      </c>
+      <c r="B1156" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1156" s="2">
+        <v>43751</v>
+      </c>
+      <c r="D1156" t="s">
+        <v>1054</v>
+      </c>
+      <c r="E1156" t="s">
+        <v>222</v>
+      </c>
+      <c r="F1156">
+        <v>5</v>
+      </c>
+      <c r="H1156" t="s">
+        <v>255</v>
+      </c>
+      <c r="I1156">
+        <v>1154</v>
+      </c>
+      <c r="J1156" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1157" spans="1:10">
+      <c r="A1157">
+        <v>5</v>
+      </c>
+      <c r="B1157" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1157" s="2">
+        <v>43752</v>
+      </c>
+      <c r="D1157" t="s">
+        <v>1053</v>
+      </c>
+      <c r="E1157" t="s">
+        <v>222</v>
+      </c>
+      <c r="F1157">
+        <v>5</v>
+      </c>
+      <c r="H1157" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1157">
+        <v>1155</v>
+      </c>
+      <c r="J1157" t="s">
+        <v>637</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Kapnogona mono re mounia
</commit_message>
<xml_diff>
--- a/DataBase/Manos costs/costs.xlsx
+++ b/DataBase/Manos costs/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5922" uniqueCount="1079">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5947" uniqueCount="1082">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -3251,6 +3251,15 @@
   </si>
   <si>
     <t>Trikala</t>
+  </si>
+  <si>
+    <t>κρουασίνια κρουασάν και coca-cola με στέβια</t>
+  </si>
+  <si>
+    <t>2 κομμάτια πίτσα χωριάτικη</t>
+  </si>
+  <si>
+    <t>2 caprice</t>
   </si>
 </sst>
 </file>
@@ -3704,10 +3713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1183"/>
+  <dimension ref="A1:L1187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1159" workbookViewId="0">
-      <selection activeCell="J1171" sqref="J1171:J1182"/>
+    <sheetView tabSelected="1" topLeftCell="D1170" workbookViewId="0">
+      <selection activeCell="I1181" sqref="I1181:I1187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -38346,7 +38355,7 @@
     </row>
     <row r="1179" spans="1:10">
       <c r="A1179">
-        <v>3.8</v>
+        <v>3.13</v>
       </c>
       <c r="B1179" t="s">
         <v>207</v>
@@ -38461,7 +38470,149 @@
       </c>
     </row>
     <row r="1183" spans="1:10">
-      <c r="C1183" s="2"/>
+      <c r="A1183">
+        <v>1</v>
+      </c>
+      <c r="B1183" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1183" s="2">
+        <v>43767</v>
+      </c>
+      <c r="D1183" t="s">
+        <v>1071</v>
+      </c>
+      <c r="E1183" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1183">
+        <v>5</v>
+      </c>
+      <c r="H1183" t="s">
+        <v>244</v>
+      </c>
+      <c r="I1183">
+        <v>1181</v>
+      </c>
+      <c r="J1183" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1184" spans="1:10">
+      <c r="A1184">
+        <v>1</v>
+      </c>
+      <c r="B1184" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1184" s="2">
+        <v>43767</v>
+      </c>
+      <c r="D1184" t="s">
+        <v>1068</v>
+      </c>
+      <c r="E1184" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1184">
+        <v>5</v>
+      </c>
+      <c r="H1184" t="s">
+        <v>244</v>
+      </c>
+      <c r="I1184">
+        <v>1182</v>
+      </c>
+      <c r="J1184" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1185" spans="1:10">
+      <c r="A1185">
+        <v>2.8</v>
+      </c>
+      <c r="B1185" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1185" s="2">
+        <v>43768</v>
+      </c>
+      <c r="D1185" t="s">
+        <v>1079</v>
+      </c>
+      <c r="E1185" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1185">
+        <v>5</v>
+      </c>
+      <c r="H1185" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1185">
+        <v>1183</v>
+      </c>
+      <c r="J1185" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="1186" spans="1:10">
+      <c r="A1186">
+        <v>3.8</v>
+      </c>
+      <c r="B1186" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1186" s="2">
+        <v>43768</v>
+      </c>
+      <c r="D1186" t="s">
+        <v>1080</v>
+      </c>
+      <c r="E1186" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1186">
+        <v>5</v>
+      </c>
+      <c r="H1186" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1186">
+        <v>1184</v>
+      </c>
+      <c r="J1186" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1187" spans="1:10">
+      <c r="A1187">
+        <v>5.09</v>
+      </c>
+      <c r="B1187" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1187" s="2">
+        <v>43768</v>
+      </c>
+      <c r="D1187" t="s">
+        <v>1081</v>
+      </c>
+      <c r="E1187" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1187">
+        <v>5</v>
+      </c>
+      <c r="H1187" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1187">
+        <v>1185</v>
+      </c>
+      <c r="J1187" t="s">
+        <v>637</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Pws kanw merge se ayto poy moy eipes, mpes instagram
</commit_message>
<xml_diff>
--- a/DataBase/Manos costs/costs.xlsx
+++ b/DataBase/Manos costs/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5982" uniqueCount="1088">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5997" uniqueCount="1090">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -3278,6 +3278,12 @@
   </si>
   <si>
     <t>Εισητήριο για τον Joker με την Ζωή Πρέντη (+ Ζωής)</t>
+  </si>
+  <si>
+    <t>κουλούρι με ελιά και τυρί, σάντουιτς με χωριάτικη και ντόνατ</t>
+  </si>
+  <si>
+    <t>πατατάκια με μπαρμπεκιου και 2 τσίχλες</t>
   </si>
 </sst>
 </file>
@@ -3731,10 +3737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1194"/>
+  <dimension ref="A1:L1197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1185" workbookViewId="0">
-      <selection activeCell="J1194" sqref="J1194"/>
+    <sheetView tabSelected="1" topLeftCell="A1185" workbookViewId="0">
+      <selection activeCell="C1198" sqref="C1198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -38835,6 +38841,93 @@
         <v>646</v>
       </c>
     </row>
+    <row r="1195" spans="1:10">
+      <c r="A1195">
+        <v>4</v>
+      </c>
+      <c r="B1195" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1195" s="2">
+        <v>43775</v>
+      </c>
+      <c r="D1195" t="s">
+        <v>1088</v>
+      </c>
+      <c r="E1195" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1195">
+        <v>5</v>
+      </c>
+      <c r="H1195" t="s">
+        <v>228</v>
+      </c>
+      <c r="I1195">
+        <v>1193</v>
+      </c>
+      <c r="J1195" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1196" spans="1:10">
+      <c r="A1196">
+        <v>1.5</v>
+      </c>
+      <c r="B1196" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1196" s="2">
+        <v>43775</v>
+      </c>
+      <c r="D1196" t="s">
+        <v>1089</v>
+      </c>
+      <c r="E1196" t="s">
+        <v>222</v>
+      </c>
+      <c r="F1196">
+        <v>5</v>
+      </c>
+      <c r="H1196" t="s">
+        <v>244</v>
+      </c>
+      <c r="I1196">
+        <v>1194</v>
+      </c>
+      <c r="J1196" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1197" spans="1:10">
+      <c r="A1197">
+        <v>1.7</v>
+      </c>
+      <c r="B1197" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1197" s="2">
+        <v>43775</v>
+      </c>
+      <c r="D1197" t="s">
+        <v>914</v>
+      </c>
+      <c r="E1197" t="s">
+        <v>222</v>
+      </c>
+      <c r="F1197">
+        <v>5</v>
+      </c>
+      <c r="H1197" t="s">
+        <v>244</v>
+      </c>
+      <c r="I1197">
+        <v>1195</v>
+      </c>
+      <c r="J1197" t="s">
+        <v>637</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Austria is amazing country
</commit_message>
<xml_diff>
--- a/DataBase/Manos costs/costs.xlsx
+++ b/DataBase/Manos costs/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6012" uniqueCount="1093">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6082" uniqueCount="1108">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -3293,6 +3293,51 @@
   </si>
   <si>
     <t>κασερόπιτα, κρουασανάκια σοκολάτας και capuccino σκέτο</t>
+  </si>
+  <si>
+    <t>goodys με Δέσποινα</t>
+  </si>
+  <si>
+    <t>monster και fruits από 7days</t>
+  </si>
+  <si>
+    <t>Exarcheia</t>
+  </si>
+  <si>
+    <t>Doukisis</t>
+  </si>
+  <si>
+    <t>εισητήριο τρένου από Βιέννη Λινζ</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>sandwich και κρουασάν σοκολάτας από super market</t>
+  </si>
+  <si>
+    <t>wok n grill (+ Σάσαρη)</t>
+  </si>
+  <si>
+    <t>souvenirs από Κρουμλοβ</t>
+  </si>
+  <si>
+    <t>σοκολατάκια</t>
+  </si>
+  <si>
+    <t>πρόστημο για συναλλαγή από ευρώ σε κορώνες</t>
+  </si>
+  <si>
+    <t>Czech</t>
+  </si>
+  <si>
+    <t>εισητήριο τρένου από Λινζ Βιέννη</t>
+  </si>
+  <si>
+    <t>εισητήριο από αεροδρόμιο</t>
+  </si>
+  <si>
+    <t>2 πίτσες μαργαρίτες</t>
   </si>
 </sst>
 </file>
@@ -3746,10 +3791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1200"/>
+  <dimension ref="A1:L1214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1185" workbookViewId="0">
-      <selection activeCell="J1201" sqref="J1201"/>
+    <sheetView tabSelected="1" topLeftCell="C1198" workbookViewId="0">
+      <selection activeCell="J1214" sqref="J1214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -39024,6 +39069,412 @@
         <v>639</v>
       </c>
     </row>
+    <row r="1201" spans="1:10">
+      <c r="A1201">
+        <v>7.7</v>
+      </c>
+      <c r="B1201" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1201" s="2">
+        <v>43779</v>
+      </c>
+      <c r="D1201" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E1201" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1201">
+        <v>5</v>
+      </c>
+      <c r="H1201" t="s">
+        <v>1095</v>
+      </c>
+      <c r="I1201">
+        <v>1199</v>
+      </c>
+      <c r="J1201" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="1202" spans="1:10">
+      <c r="A1202">
+        <v>3.2</v>
+      </c>
+      <c r="B1202" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1202" s="2">
+        <v>43780</v>
+      </c>
+      <c r="D1202" t="s">
+        <v>1094</v>
+      </c>
+      <c r="E1202" t="s">
+        <v>222</v>
+      </c>
+      <c r="F1202">
+        <v>5</v>
+      </c>
+      <c r="H1202" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1202">
+        <v>1200</v>
+      </c>
+      <c r="J1202" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1203" spans="1:10">
+      <c r="A1203">
+        <v>1</v>
+      </c>
+      <c r="B1203" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1203" s="2">
+        <v>43780</v>
+      </c>
+      <c r="D1203" t="s">
+        <v>1071</v>
+      </c>
+      <c r="E1203" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1203">
+        <v>5</v>
+      </c>
+      <c r="H1203" t="s">
+        <v>244</v>
+      </c>
+      <c r="I1203">
+        <v>1201</v>
+      </c>
+      <c r="J1203" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1204" spans="1:10">
+      <c r="A1204">
+        <v>5</v>
+      </c>
+      <c r="B1204" t="s">
+        <v>320</v>
+      </c>
+      <c r="C1204" s="2">
+        <v>43781</v>
+      </c>
+      <c r="D1204" t="s">
+        <v>957</v>
+      </c>
+      <c r="E1204" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1204">
+        <v>4</v>
+      </c>
+      <c r="H1204" t="s">
+        <v>1096</v>
+      </c>
+      <c r="I1204">
+        <v>1202</v>
+      </c>
+      <c r="J1204" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="1205" spans="1:10">
+      <c r="A1205">
+        <v>45.4</v>
+      </c>
+      <c r="B1205" t="s">
+        <v>320</v>
+      </c>
+      <c r="C1205" s="2">
+        <v>43781</v>
+      </c>
+      <c r="D1205" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E1205" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1205">
+        <v>4</v>
+      </c>
+      <c r="H1205" t="s">
+        <v>1098</v>
+      </c>
+      <c r="I1205">
+        <v>1203</v>
+      </c>
+      <c r="J1205" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1206" spans="1:10">
+      <c r="A1206">
+        <v>2</v>
+      </c>
+      <c r="B1206" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1206" s="2">
+        <v>43781</v>
+      </c>
+      <c r="D1206" t="s">
+        <v>1070</v>
+      </c>
+      <c r="E1206" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1206">
+        <v>4</v>
+      </c>
+      <c r="H1206" t="s">
+        <v>1098</v>
+      </c>
+      <c r="I1206">
+        <v>1204</v>
+      </c>
+      <c r="J1206" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1207" spans="1:10">
+      <c r="A1207">
+        <v>3.47</v>
+      </c>
+      <c r="B1207" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1207" s="2">
+        <v>43782</v>
+      </c>
+      <c r="D1207" t="s">
+        <v>1099</v>
+      </c>
+      <c r="E1207" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1207">
+        <v>5</v>
+      </c>
+      <c r="H1207" t="s">
+        <v>1098</v>
+      </c>
+      <c r="I1207">
+        <v>1205</v>
+      </c>
+      <c r="J1207" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="1208" spans="1:10">
+      <c r="A1208">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="B1208" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1208" s="2">
+        <v>43784</v>
+      </c>
+      <c r="D1208" t="s">
+        <v>1100</v>
+      </c>
+      <c r="E1208" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1208">
+        <v>5</v>
+      </c>
+      <c r="H1208" t="s">
+        <v>1098</v>
+      </c>
+      <c r="I1208">
+        <v>1206</v>
+      </c>
+      <c r="J1208" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="1209" spans="1:10">
+      <c r="A1209">
+        <v>14.27</v>
+      </c>
+      <c r="B1209" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1209" s="2">
+        <v>43786</v>
+      </c>
+      <c r="D1209" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E1209" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1209">
+        <v>5</v>
+      </c>
+      <c r="H1209" t="s">
+        <v>1104</v>
+      </c>
+      <c r="I1209">
+        <v>1207</v>
+      </c>
+      <c r="J1209" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="1210" spans="1:10">
+      <c r="A1210">
+        <v>5.7</v>
+      </c>
+      <c r="B1210" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1210" s="2">
+        <v>43786</v>
+      </c>
+      <c r="D1210" t="s">
+        <v>1102</v>
+      </c>
+      <c r="E1210" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1210">
+        <v>5</v>
+      </c>
+      <c r="H1210" t="s">
+        <v>1104</v>
+      </c>
+      <c r="I1210">
+        <v>1208</v>
+      </c>
+      <c r="J1210" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="1211" spans="1:10">
+      <c r="A1211">
+        <v>3</v>
+      </c>
+      <c r="B1211" t="s">
+        <v>330</v>
+      </c>
+      <c r="C1211" s="2">
+        <v>43786</v>
+      </c>
+      <c r="D1211" t="s">
+        <v>1103</v>
+      </c>
+      <c r="E1211" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1211">
+        <v>5</v>
+      </c>
+      <c r="H1211" t="s">
+        <v>1104</v>
+      </c>
+      <c r="I1211">
+        <v>1209</v>
+      </c>
+      <c r="J1211" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="1212" spans="1:10">
+      <c r="A1212">
+        <v>45.4</v>
+      </c>
+      <c r="B1212" t="s">
+        <v>320</v>
+      </c>
+      <c r="C1212" s="2">
+        <v>43788</v>
+      </c>
+      <c r="D1212" t="s">
+        <v>1105</v>
+      </c>
+      <c r="E1212" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1212">
+        <v>3</v>
+      </c>
+      <c r="H1212" t="s">
+        <v>1098</v>
+      </c>
+      <c r="I1212">
+        <v>1210</v>
+      </c>
+      <c r="J1212" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1213" spans="1:10">
+      <c r="A1213">
+        <v>5</v>
+      </c>
+      <c r="B1213" t="s">
+        <v>320</v>
+      </c>
+      <c r="C1213" s="2">
+        <v>43788</v>
+      </c>
+      <c r="D1213" t="s">
+        <v>1106</v>
+      </c>
+      <c r="E1213" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1213">
+        <v>4</v>
+      </c>
+      <c r="H1213" t="s">
+        <v>238</v>
+      </c>
+      <c r="I1213">
+        <v>1211</v>
+      </c>
+      <c r="J1213" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="1214" spans="1:10">
+      <c r="A1214">
+        <v>3.2</v>
+      </c>
+      <c r="B1214" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1214" s="2">
+        <v>43788</v>
+      </c>
+      <c r="D1214" t="s">
+        <v>1107</v>
+      </c>
+      <c r="E1214" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1214">
+        <v>4</v>
+      </c>
+      <c r="H1214" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1214">
+        <v>1212</v>
+      </c>
+      <c r="J1214" t="s">
+        <v>637</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Paw na parw ton kosta apo to aerodromio
</commit_message>
<xml_diff>
--- a/DataBase/Manos costs/costs.xlsx
+++ b/DataBase/Manos costs/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6102" uniqueCount="1110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6132" uniqueCount="1114">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -3344,6 +3344,18 @@
   </si>
   <si>
     <t>τσιτσιμπύρι με Σινάνη, Τσαγρή, Τσίρο, Τσιρογιάννη, Χοχτούλα</t>
+  </si>
+  <si>
+    <t>παπούτσια αθλητικά</t>
+  </si>
+  <si>
+    <t>ράψιμο τα γαμολουριά</t>
+  </si>
+  <si>
+    <t>strongbow με παρέα 8ου</t>
+  </si>
+  <si>
+    <t>Mc Donalds πατάτες και sprite</t>
   </si>
 </sst>
 </file>
@@ -3797,10 +3809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1218"/>
+  <dimension ref="A1:L1224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1198" workbookViewId="0">
-      <selection activeCell="I1213" sqref="I1213:I1218"/>
+    <sheetView tabSelected="1" topLeftCell="C1205" workbookViewId="0">
+      <selection activeCell="J1223" sqref="J1223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -39597,6 +39609,180 @@
         <v>637</v>
       </c>
     </row>
+    <row r="1219" spans="1:10">
+      <c r="A1219">
+        <v>31</v>
+      </c>
+      <c r="B1219" t="s">
+        <v>321</v>
+      </c>
+      <c r="C1219" s="2">
+        <v>43791</v>
+      </c>
+      <c r="D1219" t="s">
+        <v>1110</v>
+      </c>
+      <c r="E1219" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1219">
+        <v>5</v>
+      </c>
+      <c r="H1219" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1219">
+        <v>1217</v>
+      </c>
+      <c r="J1219" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1220" spans="1:10">
+      <c r="A1220">
+        <v>1</v>
+      </c>
+      <c r="B1220" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1220" s="2">
+        <v>43791</v>
+      </c>
+      <c r="D1220" t="s">
+        <v>1071</v>
+      </c>
+      <c r="E1220" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1220">
+        <v>5</v>
+      </c>
+      <c r="H1220" t="s">
+        <v>244</v>
+      </c>
+      <c r="I1220">
+        <v>1218</v>
+      </c>
+      <c r="J1220" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1221" spans="1:10">
+      <c r="A1221">
+        <v>5</v>
+      </c>
+      <c r="B1221" t="s">
+        <v>557</v>
+      </c>
+      <c r="C1221" s="2">
+        <v>43792</v>
+      </c>
+      <c r="D1221" t="s">
+        <v>1111</v>
+      </c>
+      <c r="E1221" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1221">
+        <v>3</v>
+      </c>
+      <c r="H1221" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1221">
+        <v>1219</v>
+      </c>
+      <c r="J1221" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1222" spans="1:10">
+      <c r="A1222">
+        <v>15</v>
+      </c>
+      <c r="B1222" t="s">
+        <v>320</v>
+      </c>
+      <c r="C1222" s="2">
+        <v>43792</v>
+      </c>
+      <c r="D1222" t="s">
+        <v>668</v>
+      </c>
+      <c r="E1222" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1222">
+        <v>4</v>
+      </c>
+      <c r="H1222" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1222">
+        <v>1220</v>
+      </c>
+      <c r="J1222" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="1223" spans="1:10">
+      <c r="A1223">
+        <v>5</v>
+      </c>
+      <c r="B1223" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1223" s="2">
+        <v>43792</v>
+      </c>
+      <c r="D1223" t="s">
+        <v>1112</v>
+      </c>
+      <c r="E1223" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1223">
+        <v>5</v>
+      </c>
+      <c r="H1223" t="s">
+        <v>229</v>
+      </c>
+      <c r="I1223">
+        <v>1221</v>
+      </c>
+      <c r="J1223" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1224" spans="1:10">
+      <c r="A1224">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B1224" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1224" s="2">
+        <v>43792</v>
+      </c>
+      <c r="D1224" t="s">
+        <v>1113</v>
+      </c>
+      <c r="E1224" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1224">
+        <v>5</v>
+      </c>
+      <c r="H1224" t="s">
+        <v>230</v>
+      </c>
+      <c r="I1224">
+        <v>1222</v>
+      </c>
+      <c r="J1224" t="s">
+        <v>637</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
xrvstaw 27, ptyxio pote
</commit_message>
<xml_diff>
--- a/DataBase/Manos costs/costs.xlsx
+++ b/DataBase/Manos costs/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6272" uniqueCount="1138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6312" uniqueCount="1144">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -3428,6 +3428,24 @@
   </si>
   <si>
     <t>μπλούζες black wolf</t>
+  </si>
+  <si>
+    <t>pizzetti ζελεδάκια και μπάρα πρωτεΐνης</t>
+  </si>
+  <si>
+    <t>μπύρα άλφα στο reunion</t>
+  </si>
+  <si>
+    <t>σπανακόπιτα και μπάρα με φυστικοβούτηρο</t>
+  </si>
+  <si>
+    <t>pancake με Νικηφόρο στο τρε</t>
+  </si>
+  <si>
+    <t>νερό Ο.Α.Κ.Α</t>
+  </si>
+  <si>
+    <t>(+ νερό Κ.Γιάννη)</t>
   </si>
 </sst>
 </file>
@@ -3882,10 +3900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1252"/>
+  <dimension ref="A1:L1260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1229" workbookViewId="0">
-      <selection activeCell="J1253" sqref="J1253"/>
+    <sheetView tabSelected="1" topLeftCell="C1237" workbookViewId="0">
+      <selection activeCell="J1261" sqref="J1261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -40668,6 +40686,238 @@
         <v>637</v>
       </c>
     </row>
+    <row r="1253" spans="1:10">
+      <c r="A1253">
+        <v>3.3</v>
+      </c>
+      <c r="B1253" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1253" s="2">
+        <v>43812</v>
+      </c>
+      <c r="D1253" t="s">
+        <v>1138</v>
+      </c>
+      <c r="E1253" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1253">
+        <v>4</v>
+      </c>
+      <c r="H1253" t="s">
+        <v>244</v>
+      </c>
+      <c r="I1253">
+        <v>1251</v>
+      </c>
+      <c r="J1253" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1254" spans="1:10">
+      <c r="A1254">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B1254" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1254" s="2">
+        <v>43812</v>
+      </c>
+      <c r="D1254" t="s">
+        <v>317</v>
+      </c>
+      <c r="E1254" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1254">
+        <v>4</v>
+      </c>
+      <c r="H1254" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1254">
+        <v>1252</v>
+      </c>
+      <c r="J1254" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1255" spans="1:10">
+      <c r="A1255">
+        <v>3</v>
+      </c>
+      <c r="B1255" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1255" s="2">
+        <v>43813</v>
+      </c>
+      <c r="D1255" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E1255" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1255">
+        <v>4</v>
+      </c>
+      <c r="H1255" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1255">
+        <v>1253</v>
+      </c>
+      <c r="J1255" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1256" spans="1:10">
+      <c r="A1256">
+        <v>3.8</v>
+      </c>
+      <c r="B1256" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1256" s="2">
+        <v>43814</v>
+      </c>
+      <c r="D1256" t="s">
+        <v>1140</v>
+      </c>
+      <c r="E1256" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1256">
+        <v>4</v>
+      </c>
+      <c r="H1256" t="s">
+        <v>865</v>
+      </c>
+      <c r="I1256">
+        <v>1254</v>
+      </c>
+      <c r="J1256" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1257" spans="1:10">
+      <c r="A1257">
+        <v>1.9</v>
+      </c>
+      <c r="B1257" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1257" s="2">
+        <v>43814</v>
+      </c>
+      <c r="D1257" t="s">
+        <v>188</v>
+      </c>
+      <c r="E1257" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1257">
+        <v>4</v>
+      </c>
+      <c r="H1257" t="s">
+        <v>244</v>
+      </c>
+      <c r="I1257">
+        <v>1255</v>
+      </c>
+      <c r="J1257" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1258" spans="1:10">
+      <c r="A1258">
+        <v>4.8</v>
+      </c>
+      <c r="B1258" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1258" s="2">
+        <v>43814</v>
+      </c>
+      <c r="D1258" t="s">
+        <v>1141</v>
+      </c>
+      <c r="E1258" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1258">
+        <v>4</v>
+      </c>
+      <c r="H1258" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1258">
+        <v>1256</v>
+      </c>
+      <c r="J1258" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1259" spans="1:10">
+      <c r="A1259">
+        <v>1</v>
+      </c>
+      <c r="B1259" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1259" s="2">
+        <v>43815</v>
+      </c>
+      <c r="D1259" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E1259" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1259">
+        <v>5</v>
+      </c>
+      <c r="H1259" t="s">
+        <v>244</v>
+      </c>
+      <c r="I1259">
+        <v>1257</v>
+      </c>
+      <c r="J1259" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1260" spans="1:10">
+      <c r="A1260">
+        <v>0.5</v>
+      </c>
+      <c r="B1260" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1260" s="2">
+        <v>43815</v>
+      </c>
+      <c r="D1260" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E1260" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1260">
+        <v>5</v>
+      </c>
+      <c r="H1260" t="s">
+        <v>244</v>
+      </c>
+      <c r="I1260">
+        <v>1258</v>
+      </c>
+      <c r="J1260" t="s">
+        <v>637</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
apla h sxoli gamietai
</commit_message>
<xml_diff>
--- a/DataBase/Manos costs/costs.xlsx
+++ b/DataBase/Manos costs/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6312" uniqueCount="1144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6322" uniqueCount="1146">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -3446,6 +3446,12 @@
   </si>
   <si>
     <t>(+ νερό Κ.Γιάννη)</t>
+  </si>
+  <si>
+    <t>sandwich και λιχναράκια από το πρώην Φουρναριό</t>
+  </si>
+  <si>
+    <t>pizza από το pizza.gr στο mall, νερό και coca-cola zero με λεμόνι</t>
   </si>
 </sst>
 </file>
@@ -3900,10 +3906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1260"/>
+  <dimension ref="A1:L1262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1237" workbookViewId="0">
-      <selection activeCell="J1261" sqref="J1261"/>
+    <sheetView tabSelected="1" topLeftCell="C1239" workbookViewId="0">
+      <selection activeCell="I1259" sqref="I1259:I1262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -40918,6 +40924,64 @@
         <v>637</v>
       </c>
     </row>
+    <row r="1261" spans="1:10">
+      <c r="A1261">
+        <v>3.7</v>
+      </c>
+      <c r="B1261" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1261" s="2">
+        <v>43816</v>
+      </c>
+      <c r="D1261" t="s">
+        <v>1144</v>
+      </c>
+      <c r="E1261" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1261">
+        <v>5</v>
+      </c>
+      <c r="H1261" t="s">
+        <v>228</v>
+      </c>
+      <c r="I1261">
+        <v>1259</v>
+      </c>
+      <c r="J1261" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="1262" spans="1:10">
+      <c r="A1262">
+        <v>7</v>
+      </c>
+      <c r="B1262" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1262" s="2">
+        <v>43816</v>
+      </c>
+      <c r="D1262" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E1262" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1262">
+        <v>5</v>
+      </c>
+      <c r="H1262" t="s">
+        <v>244</v>
+      </c>
+      <c r="I1262">
+        <v>1260</v>
+      </c>
+      <c r="J1262" t="s">
+        <v>639</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
me 18 C xristougenna den ta les
</commit_message>
<xml_diff>
--- a/DataBase/Manos costs/costs.xlsx
+++ b/DataBase/Manos costs/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6322" uniqueCount="1146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6367" uniqueCount="1154">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -3452,6 +3452,30 @@
   </si>
   <si>
     <t>pizza από το pizza.gr στο mall, νερό και coca-cola zero με λεμόνι</t>
+  </si>
+  <si>
+    <t>καφές με Τσίρο στο Soiynee tod</t>
+  </si>
+  <si>
+    <t>στοίχοιμα συναυλία</t>
+  </si>
+  <si>
+    <t>2 κουλούρια με ντομάτα και τυρί από τον Βενέτη</t>
+  </si>
+  <si>
+    <t>μπύρα με Αγγελίδη, τσίρο Μαειρίν</t>
+  </si>
+  <si>
+    <t>3 ντέρμπι από το περίπτερο στην δέγλερη</t>
+  </si>
+  <si>
+    <t>σπανακόπιτα και λιχναράκια από το Πρώην φουρναριό</t>
+  </si>
+  <si>
+    <t>5 κρουασίνια από το κυλικείο της σχολής</t>
+  </si>
+  <si>
+    <t>κρέμες στιγμής γάλα advanced και ένα χυμό ροδάκινο από τον Κρητικό</t>
   </si>
 </sst>
 </file>
@@ -3906,10 +3930,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1262"/>
+  <dimension ref="A1:L1271"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1239" workbookViewId="0">
-      <selection activeCell="I1259" sqref="I1259:I1262"/>
+    <sheetView tabSelected="1" topLeftCell="A1255" workbookViewId="0">
+      <selection activeCell="D1024" sqref="D1024"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -40982,6 +41006,267 @@
         <v>639</v>
       </c>
     </row>
+    <row r="1263" spans="1:10">
+      <c r="A1263">
+        <v>3.5</v>
+      </c>
+      <c r="B1263" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1263" s="2">
+        <v>43817</v>
+      </c>
+      <c r="D1263" t="s">
+        <v>1146</v>
+      </c>
+      <c r="E1263" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1263">
+        <v>5</v>
+      </c>
+      <c r="H1263" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1263">
+        <v>1261</v>
+      </c>
+      <c r="J1263" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1264" spans="1:10">
+      <c r="A1264">
+        <v>10</v>
+      </c>
+      <c r="B1264" t="s">
+        <v>324</v>
+      </c>
+      <c r="C1264" s="2">
+        <v>43817</v>
+      </c>
+      <c r="D1264" t="s">
+        <v>1147</v>
+      </c>
+      <c r="E1264" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1264">
+        <v>5</v>
+      </c>
+      <c r="H1264" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1264">
+        <v>1262</v>
+      </c>
+      <c r="J1264" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1265" spans="1:10">
+      <c r="A1265">
+        <v>3.3</v>
+      </c>
+      <c r="B1265" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1265" s="2">
+        <v>43818</v>
+      </c>
+      <c r="D1265" t="s">
+        <v>1148</v>
+      </c>
+      <c r="E1265" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1265">
+        <v>5</v>
+      </c>
+      <c r="H1265" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1265">
+        <v>1263</v>
+      </c>
+      <c r="J1265" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1266" spans="1:10">
+      <c r="A1266">
+        <v>3.9</v>
+      </c>
+      <c r="B1266" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1266" s="2">
+        <v>43818</v>
+      </c>
+      <c r="D1266" t="s">
+        <v>734</v>
+      </c>
+      <c r="E1266" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1266">
+        <v>5</v>
+      </c>
+      <c r="H1266" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1266">
+        <v>1264</v>
+      </c>
+      <c r="J1266" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1267" spans="1:10">
+      <c r="A1267">
+        <v>2</v>
+      </c>
+      <c r="B1267" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1267" s="2">
+        <v>43818</v>
+      </c>
+      <c r="D1267" t="s">
+        <v>1149</v>
+      </c>
+      <c r="E1267" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1267">
+        <v>5</v>
+      </c>
+      <c r="H1267" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1267">
+        <v>1265</v>
+      </c>
+      <c r="J1267" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1268" spans="1:10">
+      <c r="A1268">
+        <v>1.8</v>
+      </c>
+      <c r="B1268" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1268" s="2">
+        <v>43818</v>
+      </c>
+      <c r="D1268" t="s">
+        <v>1150</v>
+      </c>
+      <c r="E1268" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1268">
+        <v>5</v>
+      </c>
+      <c r="H1268" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1268">
+        <v>1266</v>
+      </c>
+      <c r="J1268" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1269" spans="1:10">
+      <c r="A1269">
+        <v>3</v>
+      </c>
+      <c r="B1269" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1269" s="2">
+        <v>43819</v>
+      </c>
+      <c r="D1269" t="s">
+        <v>1151</v>
+      </c>
+      <c r="E1269" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1269">
+        <v>4</v>
+      </c>
+      <c r="H1269" t="s">
+        <v>228</v>
+      </c>
+      <c r="I1269">
+        <v>1267</v>
+      </c>
+      <c r="J1269" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1270" spans="1:10">
+      <c r="A1270">
+        <v>2</v>
+      </c>
+      <c r="B1270" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1270" s="2">
+        <v>43819</v>
+      </c>
+      <c r="D1270" t="s">
+        <v>1152</v>
+      </c>
+      <c r="E1270" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1270">
+        <v>4</v>
+      </c>
+      <c r="H1270" t="s">
+        <v>228</v>
+      </c>
+      <c r="I1270">
+        <v>1268</v>
+      </c>
+      <c r="J1270" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1271" spans="1:10">
+      <c r="A1271">
+        <v>4.12</v>
+      </c>
+      <c r="B1271" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1271" s="2">
+        <v>43819</v>
+      </c>
+      <c r="D1271" t="s">
+        <v>1153</v>
+      </c>
+      <c r="E1271" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1271">
+        <v>4</v>
+      </c>
+      <c r="H1271" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1271">
+        <v>1269</v>
+      </c>
+      <c r="J1271" t="s">
+        <v>637</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
nomiza poti edina me8aurio kai dinw ayrio skataaaaa
</commit_message>
<xml_diff>
--- a/DataBase/Manos costs/costs.xlsx
+++ b/DataBase/Manos costs/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6717" uniqueCount="1219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6742" uniqueCount="1223">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -3671,6 +3671,18 @@
   </si>
   <si>
     <t>πατατάκια και Osphee</t>
+  </si>
+  <si>
+    <t>(+ βενζίνη πατέρα)</t>
+  </si>
+  <si>
+    <t>2 οικολογικά σουβλάκια (+ 2 σουβλάκια μανούλας)</t>
+  </si>
+  <si>
+    <t>sprite και bueno</t>
+  </si>
+  <si>
+    <t>μακαρονάδα, μεξικάνικη σαλάτα και κρύα σοκολάτα από efood</t>
   </si>
 </sst>
 </file>
@@ -4125,10 +4137,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1341"/>
+  <dimension ref="A1:L1346"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1325" workbookViewId="0">
-      <selection activeCell="J1328" sqref="J1328:J1341"/>
+    <sheetView tabSelected="1" topLeftCell="D1325" workbookViewId="0">
+      <selection activeCell="I1340" sqref="I1340:I1346"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -43492,6 +43504,151 @@
         <v>637</v>
       </c>
     </row>
+    <row r="1342" spans="1:10">
+      <c r="A1342">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B1342" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1342" s="2">
+        <v>43860</v>
+      </c>
+      <c r="D1342" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E1342" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1342">
+        <v>4</v>
+      </c>
+      <c r="H1342" t="s">
+        <v>244</v>
+      </c>
+      <c r="I1342">
+        <v>1340</v>
+      </c>
+      <c r="J1342" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1343" spans="1:10">
+      <c r="A1343">
+        <v>2</v>
+      </c>
+      <c r="B1343" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1343" s="2">
+        <v>43861</v>
+      </c>
+      <c r="D1343" t="s">
+        <v>1221</v>
+      </c>
+      <c r="E1343" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1343">
+        <v>4</v>
+      </c>
+      <c r="H1343" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1343">
+        <v>1341</v>
+      </c>
+      <c r="J1343" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1344" spans="1:10">
+      <c r="A1344">
+        <v>10</v>
+      </c>
+      <c r="B1344" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1344" s="2">
+        <v>43861</v>
+      </c>
+      <c r="D1344" t="s">
+        <v>1220</v>
+      </c>
+      <c r="E1344" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1344">
+        <v>4</v>
+      </c>
+      <c r="H1344" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1344">
+        <v>1342</v>
+      </c>
+      <c r="J1344" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1345" spans="1:10">
+      <c r="A1345">
+        <v>10</v>
+      </c>
+      <c r="B1345" t="s">
+        <v>320</v>
+      </c>
+      <c r="C1345" s="2">
+        <v>43865</v>
+      </c>
+      <c r="D1345" t="s">
+        <v>1219</v>
+      </c>
+      <c r="E1345" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1345">
+        <v>3</v>
+      </c>
+      <c r="H1345" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1345">
+        <v>1343</v>
+      </c>
+      <c r="J1345" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="1346" spans="1:10">
+      <c r="A1346">
+        <v>10</v>
+      </c>
+      <c r="B1346" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1346" s="2">
+        <v>43865</v>
+      </c>
+      <c r="D1346" t="s">
+        <v>1222</v>
+      </c>
+      <c r="E1346" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1346">
+        <v>3</v>
+      </c>
+      <c r="H1346" t="s">
+        <v>224</v>
+      </c>
+      <c r="I1346">
+        <v>1344</v>
+      </c>
+      <c r="J1346" t="s">
+        <v>637</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
prepei na kleisoyme gia TEDx
</commit_message>
<xml_diff>
--- a/DataBase/Manos costs/costs.xlsx
+++ b/DataBase/Manos costs/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6972" uniqueCount="1265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7012" uniqueCount="1272">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -3809,6 +3809,27 @@
   </si>
   <si>
     <t>εισιτήριο για Βέβυλο (+ Τσίρου)</t>
+  </si>
+  <si>
+    <t>(+ εφημερίδα πατέρα)</t>
+  </si>
+  <si>
+    <t>2 σοκοφρέτες</t>
+  </si>
+  <si>
+    <t>amaretti και 2 champion</t>
+  </si>
+  <si>
+    <t>2 fix ανεφ (+  Γεωργίας και Μάρκου)</t>
+  </si>
+  <si>
+    <t>νερό στο Άλσος Βεϊκου (+ Δωροθέας)</t>
+  </si>
+  <si>
+    <t>pizza margarita με Μιχάλη και Μπαρμπάκου</t>
+  </si>
+  <si>
+    <t>παπουτσια adidas</t>
   </si>
 </sst>
 </file>
@@ -4263,10 +4284,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1392"/>
+  <dimension ref="A1:L1400"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1371" workbookViewId="0">
-      <selection activeCell="I1382" sqref="I1382:I1392"/>
+    <sheetView tabSelected="1" topLeftCell="E1385" workbookViewId="0">
+      <selection activeCell="I1391" sqref="I1391:I1400"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -45109,6 +45130,238 @@
         <v>635</v>
       </c>
     </row>
+    <row r="1393" spans="1:10">
+      <c r="A1393">
+        <v>2.6</v>
+      </c>
+      <c r="B1393" t="s">
+        <v>321</v>
+      </c>
+      <c r="C1393" s="2">
+        <v>43891</v>
+      </c>
+      <c r="D1393" t="s">
+        <v>1265</v>
+      </c>
+      <c r="E1393" t="s">
+        <v>219</v>
+      </c>
+      <c r="F1393">
+        <v>4</v>
+      </c>
+      <c r="H1393" t="s">
+        <v>228</v>
+      </c>
+      <c r="I1393">
+        <v>1391</v>
+      </c>
+      <c r="J1393" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="1394" spans="1:10">
+      <c r="A1394">
+        <v>1.2</v>
+      </c>
+      <c r="B1394" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1394" s="2">
+        <v>43891</v>
+      </c>
+      <c r="D1394" t="s">
+        <v>1266</v>
+      </c>
+      <c r="E1394" t="s">
+        <v>219</v>
+      </c>
+      <c r="F1394">
+        <v>4</v>
+      </c>
+      <c r="H1394" t="s">
+        <v>228</v>
+      </c>
+      <c r="I1394">
+        <v>1392</v>
+      </c>
+      <c r="J1394" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:10">
+      <c r="A1395">
+        <v>2.6</v>
+      </c>
+      <c r="B1395" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1395" s="2">
+        <v>43891</v>
+      </c>
+      <c r="D1395" t="s">
+        <v>1267</v>
+      </c>
+      <c r="E1395" t="s">
+        <v>219</v>
+      </c>
+      <c r="F1395">
+        <v>4</v>
+      </c>
+      <c r="H1395" t="s">
+        <v>222</v>
+      </c>
+      <c r="I1395">
+        <v>1393</v>
+      </c>
+      <c r="J1395" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:10">
+      <c r="A1396">
+        <v>21</v>
+      </c>
+      <c r="B1396" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1396" s="2">
+        <v>43891</v>
+      </c>
+      <c r="D1396" t="s">
+        <v>1268</v>
+      </c>
+      <c r="E1396" t="s">
+        <v>219</v>
+      </c>
+      <c r="F1396">
+        <v>5</v>
+      </c>
+      <c r="H1396" t="s">
+        <v>228</v>
+      </c>
+      <c r="I1396">
+        <v>1394</v>
+      </c>
+      <c r="J1396" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="1397" spans="1:10">
+      <c r="A1397">
+        <v>1</v>
+      </c>
+      <c r="B1397" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1397" s="2">
+        <v>43892</v>
+      </c>
+      <c r="D1397" t="s">
+        <v>1269</v>
+      </c>
+      <c r="E1397" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1397">
+        <v>5</v>
+      </c>
+      <c r="H1397" t="s">
+        <v>251</v>
+      </c>
+      <c r="I1397">
+        <v>1395</v>
+      </c>
+      <c r="J1397" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:10">
+      <c r="A1398">
+        <v>0.8</v>
+      </c>
+      <c r="B1398" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1398" s="2">
+        <v>43892</v>
+      </c>
+      <c r="D1398" t="s">
+        <v>293</v>
+      </c>
+      <c r="E1398" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1398">
+        <v>5</v>
+      </c>
+      <c r="H1398" t="s">
+        <v>251</v>
+      </c>
+      <c r="I1398">
+        <v>1396</v>
+      </c>
+      <c r="J1398" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:10">
+      <c r="A1399">
+        <v>6</v>
+      </c>
+      <c r="B1399" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1399" s="2">
+        <v>43892</v>
+      </c>
+      <c r="D1399" t="s">
+        <v>1270</v>
+      </c>
+      <c r="E1399" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1399">
+        <v>5</v>
+      </c>
+      <c r="H1399" t="s">
+        <v>225</v>
+      </c>
+      <c r="I1399">
+        <v>1397</v>
+      </c>
+      <c r="J1399" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:10">
+      <c r="A1400">
+        <v>45</v>
+      </c>
+      <c r="B1400" t="s">
+        <v>319</v>
+      </c>
+      <c r="C1400" s="2">
+        <v>43893</v>
+      </c>
+      <c r="D1400" t="s">
+        <v>1271</v>
+      </c>
+      <c r="E1400" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1400">
+        <v>5</v>
+      </c>
+      <c r="H1400" t="s">
+        <v>222</v>
+      </c>
+      <c r="I1400">
+        <v>1398</v>
+      </c>
+      <c r="J1400" t="s">
+        <v>642</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
kalitera poy den ir8es sto TEDx
</commit_message>
<xml_diff>
--- a/DataBase/Manos costs/costs.xlsx
+++ b/DataBase/Manos costs/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7012" uniqueCount="1272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7067" uniqueCount="1281">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -3830,6 +3830,33 @@
   </si>
   <si>
     <t>παπουτσια adidas</t>
+  </si>
+  <si>
+    <t>παπούτσια δίσκου και μπάλα στον Φλοίσβο</t>
+  </si>
+  <si>
+    <t>καφές στον Φλοίσβο</t>
+  </si>
+  <si>
+    <t>τρένο για Λάρισα για το TEDx</t>
+  </si>
+  <si>
+    <t>οφθαλμίαρτος</t>
+  </si>
+  <si>
+    <t>supermarket μπισκότα και τσίχλες</t>
+  </si>
+  <si>
+    <t>εισιτήριο για ΤΕΙ</t>
+  </si>
+  <si>
+    <t>ice tea</t>
+  </si>
+  <si>
+    <t>taxi από σταθμο λαρίσης περιστέρι</t>
+  </si>
+  <si>
+    <t>πατατάκια νερό και bueno</t>
   </si>
 </sst>
 </file>
@@ -4284,10 +4311,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1400"/>
+  <dimension ref="A1:L1411"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1385" workbookViewId="0">
-      <selection activeCell="I1391" sqref="I1391:I1400"/>
+    <sheetView tabSelected="1" topLeftCell="F1399" workbookViewId="0">
+      <selection activeCell="J1412" sqref="J1412"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -45362,6 +45389,325 @@
         <v>642</v>
       </c>
     </row>
+    <row r="1401" spans="1:10">
+      <c r="A1401">
+        <v>1.5</v>
+      </c>
+      <c r="B1401" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1401" s="2">
+        <v>43893</v>
+      </c>
+      <c r="D1401" t="s">
+        <v>1058</v>
+      </c>
+      <c r="E1401" t="s">
+        <v>218</v>
+      </c>
+      <c r="F1401">
+        <v>5</v>
+      </c>
+      <c r="H1401" t="s">
+        <v>242</v>
+      </c>
+      <c r="I1401">
+        <v>1399</v>
+      </c>
+      <c r="J1401" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:10">
+      <c r="A1402">
+        <v>85.5</v>
+      </c>
+      <c r="B1402" t="s">
+        <v>319</v>
+      </c>
+      <c r="C1402" s="2">
+        <v>43894</v>
+      </c>
+      <c r="D1402" t="s">
+        <v>1272</v>
+      </c>
+      <c r="E1402" t="s">
+        <v>218</v>
+      </c>
+      <c r="F1402">
+        <v>5</v>
+      </c>
+      <c r="H1402" t="s">
+        <v>226</v>
+      </c>
+      <c r="I1402">
+        <v>1400</v>
+      </c>
+      <c r="J1402" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:10">
+      <c r="A1403">
+        <v>4.2</v>
+      </c>
+      <c r="B1403" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1403" s="2">
+        <v>43894</v>
+      </c>
+      <c r="D1403" t="s">
+        <v>1273</v>
+      </c>
+      <c r="E1403" t="s">
+        <v>218</v>
+      </c>
+      <c r="F1403">
+        <v>5</v>
+      </c>
+      <c r="H1403" t="s">
+        <v>226</v>
+      </c>
+      <c r="I1403">
+        <v>1401</v>
+      </c>
+      <c r="J1403" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:10">
+      <c r="A1404">
+        <v>35.1</v>
+      </c>
+      <c r="B1404" t="s">
+        <v>318</v>
+      </c>
+      <c r="C1404" s="2">
+        <v>43896</v>
+      </c>
+      <c r="D1404" t="s">
+        <v>1274</v>
+      </c>
+      <c r="E1404" t="s">
+        <v>218</v>
+      </c>
+      <c r="F1404">
+        <v>5</v>
+      </c>
+      <c r="H1404" t="s">
+        <v>222</v>
+      </c>
+      <c r="I1404">
+        <v>1402</v>
+      </c>
+      <c r="J1404" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:10">
+      <c r="A1405">
+        <v>10</v>
+      </c>
+      <c r="B1405" t="s">
+        <v>320</v>
+      </c>
+      <c r="C1405" s="2">
+        <v>43896</v>
+      </c>
+      <c r="D1405" t="s">
+        <v>1275</v>
+      </c>
+      <c r="E1405" t="s">
+        <v>218</v>
+      </c>
+      <c r="F1405">
+        <v>5</v>
+      </c>
+      <c r="H1405" t="s">
+        <v>222</v>
+      </c>
+      <c r="I1405">
+        <v>1403</v>
+      </c>
+      <c r="J1405" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:10">
+      <c r="A1406">
+        <v>0.5</v>
+      </c>
+      <c r="B1406" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1406" s="2">
+        <v>43896</v>
+      </c>
+      <c r="D1406" t="s">
+        <v>1127</v>
+      </c>
+      <c r="E1406" t="s">
+        <v>218</v>
+      </c>
+      <c r="F1406">
+        <v>5</v>
+      </c>
+      <c r="H1406" t="s">
+        <v>242</v>
+      </c>
+      <c r="I1406">
+        <v>1404</v>
+      </c>
+      <c r="J1406" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:10">
+      <c r="A1407">
+        <v>8.86</v>
+      </c>
+      <c r="B1407" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1407" s="2">
+        <v>43896</v>
+      </c>
+      <c r="D1407" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E1407" t="s">
+        <v>218</v>
+      </c>
+      <c r="F1407">
+        <v>5</v>
+      </c>
+      <c r="H1407" t="s">
+        <v>222</v>
+      </c>
+      <c r="I1407">
+        <v>1405</v>
+      </c>
+      <c r="J1407" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="1408" spans="1:10">
+      <c r="A1408">
+        <v>0.6</v>
+      </c>
+      <c r="B1408" t="s">
+        <v>318</v>
+      </c>
+      <c r="C1408" s="2">
+        <v>43897</v>
+      </c>
+      <c r="D1408" t="s">
+        <v>1277</v>
+      </c>
+      <c r="E1408" t="s">
+        <v>218</v>
+      </c>
+      <c r="F1408">
+        <v>4</v>
+      </c>
+      <c r="H1408" t="s">
+        <v>1253</v>
+      </c>
+      <c r="I1408">
+        <v>1406</v>
+      </c>
+      <c r="J1408" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="1409" spans="1:10">
+      <c r="A1409">
+        <v>1.2</v>
+      </c>
+      <c r="B1409" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1409" s="2">
+        <v>43897</v>
+      </c>
+      <c r="D1409" t="s">
+        <v>1278</v>
+      </c>
+      <c r="E1409" t="s">
+        <v>218</v>
+      </c>
+      <c r="F1409">
+        <v>4</v>
+      </c>
+      <c r="H1409" t="s">
+        <v>1253</v>
+      </c>
+      <c r="I1409">
+        <v>1407</v>
+      </c>
+      <c r="J1409" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="1410" spans="1:10">
+      <c r="A1410">
+        <v>4</v>
+      </c>
+      <c r="B1410" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1410" s="2">
+        <v>43898</v>
+      </c>
+      <c r="D1410" t="s">
+        <v>1280</v>
+      </c>
+      <c r="E1410" t="s">
+        <v>218</v>
+      </c>
+      <c r="F1410">
+        <v>2</v>
+      </c>
+      <c r="H1410" t="s">
+        <v>1253</v>
+      </c>
+      <c r="I1410">
+        <v>1408</v>
+      </c>
+      <c r="J1410" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="1411" spans="1:10">
+      <c r="A1411">
+        <v>8.5</v>
+      </c>
+      <c r="B1411" t="s">
+        <v>318</v>
+      </c>
+      <c r="C1411" s="2">
+        <v>43898</v>
+      </c>
+      <c r="D1411" t="s">
+        <v>1279</v>
+      </c>
+      <c r="E1411" t="s">
+        <v>218</v>
+      </c>
+      <c r="F1411">
+        <v>3</v>
+      </c>
+      <c r="H1411" t="s">
+        <v>222</v>
+      </c>
+      <c r="I1411">
+        <v>1409</v>
+      </c>
+      <c r="J1411" t="s">
+        <v>633</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>